<commit_message>
added Anforderungen and created an KiCad file
</commit_message>
<xml_diff>
--- a/Zeitplan_Anforderungen/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
+++ b/Zeitplan_Anforderungen/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4b8c2adf92642a/Berufsschule/BuP/5_Semester/Marvin/Zeitplan_Anforderungen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FE8D907-79C8-4D2A-8F1E-9B2D60FBCFC3}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87ECBD5B-1CBC-4F2B-A508-5F60621592ED}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="89">
   <si>
     <t>Zeitplan</t>
   </si>
@@ -313,30 +313,15 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Das ich am Input des Audio Prints 3.3V habe</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Das am Output des Audio Prints 50db ±10db heraus gebe</t>
-  </si>
-  <si>
-    <t>Dass wenn niemand durch die Türe läuft die Batterie einen Minimalen verbrauch hat</t>
-  </si>
-  <si>
     <t>UNFUNKTIONALE ANFORDERUNGEN</t>
   </si>
   <si>
     <t>Das ich den Audio Print oberhalb der Türe montieren kann</t>
   </si>
   <si>
-    <t>Das die Gehäuse so klein wie möglichst sind</t>
-  </si>
-  <si>
-    <t>Das die Gehäuse eine möglichst ähnliche Farbe haben</t>
-  </si>
-  <si>
     <t>Das ich den Sensor Print an den Oberen Türrahmen monitieren kann (Wenn Infrarot Sensor)</t>
   </si>
   <si>
@@ -344,6 +329,78 @@
   </si>
   <si>
     <t>Dass Batterie nicht wircklich sichtbar ist</t>
+  </si>
+  <si>
+    <t>Das die Gehäuse so klein wie möglich sind</t>
+  </si>
+  <si>
+    <t>Das die Gehäuse eine möglichst ähnliche Farbe haben wie die Wand</t>
+  </si>
+  <si>
+    <t>Auf der Platine des Sensors ein Kleines Motiv von Marvin ist (aus Hitchhickers guide to the galaxy)</t>
+  </si>
+  <si>
+    <t>Die audio anlage soll mit einem Sensor ausgestattet sein, der bei annäherung oder Durchquerung aktiviert wird (Infrarot  oder Lichtschranken)</t>
+  </si>
+  <si>
+    <t>Der Sensor soll selbst aufgenommene Audiosignale auslösen</t>
+  </si>
+  <si>
+    <t>Es sollen audiodateien in verschiedenen Formaten abgespielt werden können (MP3, WAV)</t>
+  </si>
+  <si>
+    <t>Jede Aktivierung des Sensors soll nur eine Audiodatei abspielen.</t>
+  </si>
+  <si>
+    <t>Die Audio datei soll vom Benutzer auf das System geladen werden können.</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll die Audiodatei über eine SD-Karte auf das System hochladen können.</t>
+  </si>
+  <si>
+    <t>Die Lautstärke soll physisch eingestellt werden können (Regler oder Tasten)</t>
+  </si>
+  <si>
+    <t>Eine LED soll anzeigen ob der Sensor ein Signal gegeben hat.</t>
+  </si>
+  <si>
+    <t>Die Lautstärke soll nach dem Ausschalten der Anlage gespeichert werden</t>
+  </si>
+  <si>
+    <t>Am Output des Audio Prints sollen 50db ±10db heraus gegeben werden.</t>
+  </si>
+  <si>
+    <t>Am Input des Audio Prints soll ich nicht mehr als 3.3V haben.</t>
+  </si>
+  <si>
+    <t>Der Sensor soll nach 0,5 Sekunder nach Annäherung oder Durchquerung reagieren.</t>
+  </si>
+  <si>
+    <t>Die Anlage soll im Standby-Modus einen minimalen Stromverbrauch haben.</t>
+  </si>
+  <si>
+    <t>Es soll einen Schutzmechanismus gegen Überspannung und Kurzschluss haben.</t>
+  </si>
+  <si>
+    <t>Das System soll nach erfolgreicher Aktivierung eine kurze akustische Bestätigung abspielen, bevor die eigenltiche Audiodatei gestartet wird. (Beep)</t>
+  </si>
+  <si>
+    <t>Die Auidioanlage soll nach einer bestimmten Zeit der Inaktivität automatisch in den Stanby-Modus versetzt werden.</t>
+  </si>
+  <si>
+    <t>Es soll eine Zeitschalterfunktion geben, mit der due Anlage zu einer bestimmten Uhrzeit aktiviert wird.</t>
+  </si>
+  <si>
+    <t>Es sollen verschiedene Wiedergabeodi geben</t>
+  </si>
+  <si>
+    <t>1. Einzelwiedergabe: wird nur eine datei abgespielt</t>
+  </si>
+  <si>
+    <t>2. Zufallswiedergabe: nach aktivierung wir d eine zufällige Audiodatei abgespielt</t>
+  </si>
+  <si>
+    <t>3. Serienwiedergsabe: Nach Aktivierung werden nacheinander 2 Audiodateien abgespielt.</t>
   </si>
 </sst>
 </file>
@@ -837,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -873,19 +930,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -897,32 +960,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -945,6 +1002,20 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -966,6 +1037,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1297,195 +1372,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:143" ht="18.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:143" ht="15" thickBot="1"/>
     <row r="3" spans="1:143" ht="15" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="38" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="38" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="38" t="s">
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="42"/>
+      <c r="X3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="38" t="s">
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AF3" s="39"/>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="39"/>
-      <c r="AJ3" s="39"/>
-      <c r="AK3" s="40"/>
-      <c r="AL3" s="38" t="s">
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="41"/>
+      <c r="AH3" s="41"/>
+      <c r="AI3" s="41"/>
+      <c r="AJ3" s="41"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="AM3" s="39"/>
-      <c r="AN3" s="39"/>
-      <c r="AO3" s="39"/>
-      <c r="AP3" s="39"/>
-      <c r="AQ3" s="39"/>
-      <c r="AR3" s="40"/>
-      <c r="AS3" s="38" t="s">
+      <c r="AM3" s="41"/>
+      <c r="AN3" s="41"/>
+      <c r="AO3" s="41"/>
+      <c r="AP3" s="41"/>
+      <c r="AQ3" s="41"/>
+      <c r="AR3" s="42"/>
+      <c r="AS3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="AT3" s="39"/>
-      <c r="AU3" s="39"/>
-      <c r="AV3" s="39"/>
-      <c r="AW3" s="39"/>
-      <c r="AX3" s="39"/>
-      <c r="AY3" s="40"/>
-      <c r="AZ3" s="38" t="s">
+      <c r="AT3" s="41"/>
+      <c r="AU3" s="41"/>
+      <c r="AV3" s="41"/>
+      <c r="AW3" s="41"/>
+      <c r="AX3" s="41"/>
+      <c r="AY3" s="42"/>
+      <c r="AZ3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="BA3" s="39"/>
-      <c r="BB3" s="39"/>
-      <c r="BC3" s="39"/>
-      <c r="BD3" s="39"/>
-      <c r="BE3" s="39"/>
-      <c r="BF3" s="40"/>
-      <c r="BG3" s="38" t="s">
+      <c r="BA3" s="41"/>
+      <c r="BB3" s="41"/>
+      <c r="BC3" s="41"/>
+      <c r="BD3" s="41"/>
+      <c r="BE3" s="41"/>
+      <c r="BF3" s="42"/>
+      <c r="BG3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="BH3" s="39"/>
-      <c r="BI3" s="39"/>
-      <c r="BJ3" s="39"/>
-      <c r="BK3" s="39"/>
-      <c r="BL3" s="39"/>
-      <c r="BM3" s="40"/>
-      <c r="BN3" s="38" t="s">
+      <c r="BH3" s="41"/>
+      <c r="BI3" s="41"/>
+      <c r="BJ3" s="41"/>
+      <c r="BK3" s="41"/>
+      <c r="BL3" s="41"/>
+      <c r="BM3" s="42"/>
+      <c r="BN3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="BO3" s="39"/>
-      <c r="BP3" s="39"/>
-      <c r="BQ3" s="39"/>
-      <c r="BR3" s="39"/>
-      <c r="BS3" s="39"/>
-      <c r="BT3" s="40"/>
-      <c r="BU3" s="38" t="s">
+      <c r="BO3" s="41"/>
+      <c r="BP3" s="41"/>
+      <c r="BQ3" s="41"/>
+      <c r="BR3" s="41"/>
+      <c r="BS3" s="41"/>
+      <c r="BT3" s="42"/>
+      <c r="BU3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="BV3" s="39"/>
-      <c r="BW3" s="39"/>
-      <c r="BX3" s="39"/>
-      <c r="BY3" s="39"/>
-      <c r="BZ3" s="39"/>
-      <c r="CA3" s="40"/>
-      <c r="CB3" s="38" t="s">
+      <c r="BV3" s="41"/>
+      <c r="BW3" s="41"/>
+      <c r="BX3" s="41"/>
+      <c r="BY3" s="41"/>
+      <c r="BZ3" s="41"/>
+      <c r="CA3" s="42"/>
+      <c r="CB3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="CC3" s="39"/>
-      <c r="CD3" s="39"/>
-      <c r="CE3" s="39"/>
-      <c r="CF3" s="39"/>
-      <c r="CG3" s="39"/>
-      <c r="CH3" s="40"/>
-      <c r="CI3" s="38" t="s">
+      <c r="CC3" s="41"/>
+      <c r="CD3" s="41"/>
+      <c r="CE3" s="41"/>
+      <c r="CF3" s="41"/>
+      <c r="CG3" s="41"/>
+      <c r="CH3" s="42"/>
+      <c r="CI3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="CJ3" s="39"/>
-      <c r="CK3" s="39"/>
-      <c r="CL3" s="39"/>
-      <c r="CM3" s="39"/>
-      <c r="CN3" s="39"/>
-      <c r="CO3" s="40"/>
-      <c r="CP3" s="38" t="s">
+      <c r="CJ3" s="41"/>
+      <c r="CK3" s="41"/>
+      <c r="CL3" s="41"/>
+      <c r="CM3" s="41"/>
+      <c r="CN3" s="41"/>
+      <c r="CO3" s="42"/>
+      <c r="CP3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="CQ3" s="39"/>
-      <c r="CR3" s="39"/>
-      <c r="CS3" s="39"/>
-      <c r="CT3" s="39"/>
-      <c r="CU3" s="39"/>
-      <c r="CV3" s="40"/>
-      <c r="CW3" s="38" t="s">
+      <c r="CQ3" s="41"/>
+      <c r="CR3" s="41"/>
+      <c r="CS3" s="41"/>
+      <c r="CT3" s="41"/>
+      <c r="CU3" s="41"/>
+      <c r="CV3" s="42"/>
+      <c r="CW3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="CX3" s="39"/>
-      <c r="CY3" s="39"/>
-      <c r="CZ3" s="39"/>
-      <c r="DA3" s="39"/>
-      <c r="DB3" s="39"/>
-      <c r="DC3" s="40"/>
-      <c r="DD3" s="38" t="s">
+      <c r="CX3" s="41"/>
+      <c r="CY3" s="41"/>
+      <c r="CZ3" s="41"/>
+      <c r="DA3" s="41"/>
+      <c r="DB3" s="41"/>
+      <c r="DC3" s="42"/>
+      <c r="DD3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="DE3" s="39"/>
-      <c r="DF3" s="39"/>
-      <c r="DG3" s="39"/>
-      <c r="DH3" s="39"/>
-      <c r="DI3" s="39"/>
-      <c r="DJ3" s="40"/>
-      <c r="DK3" s="38" t="s">
+      <c r="DE3" s="41"/>
+      <c r="DF3" s="41"/>
+      <c r="DG3" s="41"/>
+      <c r="DH3" s="41"/>
+      <c r="DI3" s="41"/>
+      <c r="DJ3" s="42"/>
+      <c r="DK3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="DL3" s="39"/>
-      <c r="DM3" s="39"/>
-      <c r="DN3" s="39"/>
-      <c r="DO3" s="39"/>
-      <c r="DP3" s="39"/>
-      <c r="DQ3" s="40"/>
-      <c r="DR3" s="38" t="s">
+      <c r="DL3" s="41"/>
+      <c r="DM3" s="41"/>
+      <c r="DN3" s="41"/>
+      <c r="DO3" s="41"/>
+      <c r="DP3" s="41"/>
+      <c r="DQ3" s="42"/>
+      <c r="DR3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="DS3" s="39"/>
-      <c r="DT3" s="39"/>
-      <c r="DU3" s="39"/>
-      <c r="DV3" s="39"/>
-      <c r="DW3" s="39"/>
-      <c r="DX3" s="40"/>
-      <c r="DY3" s="33" t="s">
+      <c r="DS3" s="41"/>
+      <c r="DT3" s="41"/>
+      <c r="DU3" s="41"/>
+      <c r="DV3" s="41"/>
+      <c r="DW3" s="41"/>
+      <c r="DX3" s="42"/>
+      <c r="DY3" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="DZ3" s="34"/>
-      <c r="EA3" s="34"/>
-      <c r="EB3" s="34"/>
-      <c r="EC3" s="34"/>
-      <c r="ED3" s="34"/>
-      <c r="EE3" s="35"/>
-      <c r="EF3" s="33" t="s">
+      <c r="DZ3" s="47"/>
+      <c r="EA3" s="47"/>
+      <c r="EB3" s="47"/>
+      <c r="EC3" s="47"/>
+      <c r="ED3" s="47"/>
+      <c r="EE3" s="48"/>
+      <c r="EF3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="EG3" s="34"/>
-      <c r="EH3" s="34"/>
-      <c r="EI3" s="34"/>
-      <c r="EJ3" s="34"/>
-      <c r="EK3" s="34"/>
-      <c r="EL3" s="35"/>
+      <c r="EG3" s="47"/>
+      <c r="EH3" s="47"/>
+      <c r="EI3" s="47"/>
+      <c r="EJ3" s="47"/>
+      <c r="EK3" s="47"/>
+      <c r="EL3" s="48"/>
     </row>
     <row r="4" spans="1:143" ht="15" thickBot="1">
       <c r="A4" s="9"/>
@@ -1913,7 +1988,7 @@
       <c r="EM4" s="19"/>
     </row>
     <row r="5" spans="1:143">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="49" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -2061,7 +2136,7 @@
       <c r="EL5" s="11"/>
     </row>
     <row r="6" spans="1:143" ht="15" thickBot="1">
-      <c r="A6" s="42"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
@@ -2207,7 +2282,7 @@
       <c r="EL6" s="5"/>
     </row>
     <row r="7" spans="1:143">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -2363,7 +2438,7 @@
       <c r="EL7" s="5"/>
     </row>
     <row r="8" spans="1:143" ht="15" thickBot="1">
-      <c r="A8" s="37"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -2509,7 +2584,7 @@
       <c r="EL8" s="5"/>
     </row>
     <row r="9" spans="1:143">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -2663,7 +2738,7 @@
       <c r="EL9" s="5"/>
     </row>
     <row r="10" spans="1:143" ht="15" thickBot="1">
-      <c r="A10" s="42"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -2809,7 +2884,7 @@
       <c r="EL10" s="5"/>
     </row>
     <row r="11" spans="1:143">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -2975,7 +3050,7 @@
       <c r="EL11" s="5"/>
     </row>
     <row r="12" spans="1:143" ht="15" thickBot="1">
-      <c r="A12" s="48"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -3121,7 +3196,7 @@
       <c r="EL12" s="5"/>
     </row>
     <row r="13" spans="1:143">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="21" t="s">
@@ -3293,7 +3368,7 @@
       <c r="EL13" s="5"/>
     </row>
     <row r="14" spans="1:143" ht="15" thickBot="1">
-      <c r="A14" s="37"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
@@ -3439,7 +3514,7 @@
       <c r="EL14" s="5"/>
     </row>
     <row r="15" spans="1:143">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -3611,7 +3686,7 @@
       <c r="EL15" s="5"/>
     </row>
     <row r="16" spans="1:143" ht="15" thickBot="1">
-      <c r="A16" s="37"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -3757,7 +3832,7 @@
       <c r="EL16" s="13"/>
     </row>
     <row r="17" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -3921,7 +3996,7 @@
       <c r="EL17" s="5"/>
     </row>
     <row r="18" spans="1:142" ht="15" thickBot="1">
-      <c r="A18" s="37"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
@@ -4221,7 +4296,7 @@
       <c r="EL19" s="5"/>
     </row>
     <row r="20" spans="1:142" ht="15" thickBot="1">
-      <c r="A20" s="49"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -4521,7 +4596,7 @@
       <c r="EL21" s="5"/>
     </row>
     <row r="22" spans="1:142" ht="15" thickBot="1">
-      <c r="A22" s="49"/>
+      <c r="A22" s="45"/>
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
@@ -4847,7 +4922,7 @@
       <c r="EL23" s="5"/>
     </row>
     <row r="24" spans="1:142" ht="15" thickBot="1">
-      <c r="A24" s="49"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
@@ -5157,7 +5232,7 @@
       <c r="EL25" s="5"/>
     </row>
     <row r="26" spans="1:142" ht="15" thickBot="1">
-      <c r="A26" s="49"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
@@ -5600,23 +5675,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="DD3:DJ3"/>
-    <mergeCell ref="CW3:DC3"/>
-    <mergeCell ref="CP3:CV3"/>
-    <mergeCell ref="CI3:CO3"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="AL3:AR3"/>
-    <mergeCell ref="AE3:AK3"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
     <mergeCell ref="EF3:EL3"/>
     <mergeCell ref="DY3:EE3"/>
     <mergeCell ref="A7:A8"/>
@@ -5633,6 +5691,23 @@
     <mergeCell ref="AS3:AY3"/>
     <mergeCell ref="DR3:DX3"/>
     <mergeCell ref="DK3:DQ3"/>
+    <mergeCell ref="DD3:DJ3"/>
+    <mergeCell ref="CW3:DC3"/>
+    <mergeCell ref="CP3:CV3"/>
+    <mergeCell ref="CI3:CO3"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="AL3:AR3"/>
+    <mergeCell ref="AE3:AK3"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5644,13 +5719,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FF6EFD-F608-4DA6-AB00-E35874012156}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="80.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19">
@@ -5746,10 +5821,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5757,156 +5832,186 @@
         <v>2</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="29">
         <v>3</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>62</v>
+      <c r="B18" s="30" t="s">
+        <v>75</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="30">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29">
+      <c r="A19" s="61">
         <v>4</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30" t="s">
-        <v>60</v>
+      <c r="B19" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="29">
         <v>5</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29" t="s">
-        <v>60</v>
+      <c r="B20" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="58" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="30">
         <v>6</v>
       </c>
-      <c r="B21" s="30"/>
+      <c r="B21" s="30" t="s">
+        <v>70</v>
+      </c>
       <c r="C21" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="29">
         <v>7</v>
       </c>
-      <c r="B22" s="31"/>
+      <c r="B22" s="31" t="s">
+        <v>71</v>
+      </c>
       <c r="C22" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="30">
         <v>8</v>
       </c>
-      <c r="B23" s="32"/>
+      <c r="B23" s="32" t="s">
+        <v>72</v>
+      </c>
       <c r="C23" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="29">
         <v>9</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C24" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="30">
         <v>10</v>
       </c>
-      <c r="B25" s="30"/>
+      <c r="B25" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="C25" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="29">
         <v>11</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="29" t="s">
+        <v>74</v>
+      </c>
       <c r="C26" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="30">
         <v>12</v>
       </c>
-      <c r="B27" s="30"/>
+      <c r="B27" s="30" t="s">
+        <v>76</v>
+      </c>
       <c r="C27" s="30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="29">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="29">
+      <c r="A28" s="58">
         <v>13</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="30">
+      <c r="B28" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29">
+      <c r="A29" s="61">
         <v>14</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30" t="s">
-        <v>60</v>
+      <c r="B29" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="29">
         <v>15</v>
       </c>
-      <c r="B30" s="29"/>
+      <c r="B30" s="30" t="s">
+        <v>85</v>
+      </c>
       <c r="C30" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="30">
         <v>16</v>
       </c>
-      <c r="B31" s="30"/>
+      <c r="B31" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="C31" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="29">
         <v>17</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="29" t="s">
+        <v>87</v>
+      </c>
       <c r="C32" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="30">
         <v>18</v>
       </c>
-      <c r="B33" s="30"/>
+      <c r="B33" s="30" t="s">
+        <v>88</v>
+      </c>
       <c r="C33" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -5915,7 +6020,7 @@
       </c>
       <c r="B34" s="29"/>
       <c r="C34" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -5924,7 +6029,7 @@
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -5933,7 +6038,7 @@
       </c>
       <c r="B36" s="29"/>
       <c r="C36" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -5942,7 +6047,7 @@
       </c>
       <c r="B37" s="30"/>
       <c r="C37" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -5952,7 +6057,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="52" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
@@ -5973,10 +6078,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -5987,7 +6092,7 @@
         <v>65</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -5998,7 +6103,7 @@
         <v>66</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -6006,10 +6111,10 @@
         <v>4</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -6017,10 +6122,10 @@
         <v>5</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -6028,46 +6133,54 @@
         <v>6</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="29">
         <v>7</v>
       </c>
-      <c r="B51" s="29"/>
+      <c r="B51" s="29" t="s">
+        <v>67</v>
+      </c>
       <c r="C51" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="30">
         <v>8</v>
       </c>
-      <c r="B52" s="30"/>
+      <c r="B52" s="62" t="s">
+        <v>79</v>
+      </c>
       <c r="C52" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="29">
         <v>9</v>
       </c>
-      <c r="B53" s="29"/>
+      <c r="B53" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="C53" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="30">
         <v>10</v>
       </c>
-      <c r="B54" s="30"/>
+      <c r="B54" s="30" t="s">
+        <v>81</v>
+      </c>
       <c r="C54" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -6076,7 +6189,7 @@
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:3">

</xml_diff>

<commit_message>
updatete Zeitplan and added some of the Requirements
</commit_message>
<xml_diff>
--- a/Zeitplan_Anforderungen/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
+++ b/Zeitplan_Anforderungen/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4b8c2adf92642a/Berufsschule/BuP/5_Semester/Marvin/Zeitplan_Anforderungen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87ECBD5B-1CBC-4F2B-A508-5F60621592ED}"/>
+  <xr:revisionPtr revIDLastSave="433" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F603C4F-5F6E-40F3-A67A-5376AC307DCF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="89">
   <si>
     <t>Zeitplan</t>
   </si>
@@ -160,12 +160,6 @@
   </si>
   <si>
     <t>Blockschaltbild</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>0.5h</t>
   </si>
   <si>
     <t>REQUIREMENTS</t>
@@ -402,6 +396,12 @@
   <si>
     <t>3. Serienwiedergsabe: Nach Aktivierung werden nacheinander 2 Audiodateien abgespielt.</t>
   </si>
+  <si>
+    <t>Geplante Zeit</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
 </sst>
 </file>
 
@@ -455,18 +455,12 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7F9FF9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -484,6 +478,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F9FF9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -894,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -915,21 +921,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1002,20 +1019,21 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1024,8 +1042,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7F9FF9"/>
       <color rgb="FFD49AFC"/>
-      <color rgb="FF7F9FF9"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1362,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8C9801-39B9-4B26-94D0-9F2F7C9746D6}">
   <dimension ref="A1:EM28"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="17" workbookViewId="0">
-      <selection activeCell="AW15" sqref="AW15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="49" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1372,199 +1390,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:143" ht="18.5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:143" ht="15" thickBot="1"/>
     <row r="3" spans="1:143" ht="15" thickBot="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="40" t="s">
+      <c r="A3" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="2">
+        <f>SUM(EG27,DY25:EF25,EA23:EB23,K6:DX6,D7:G7,K9:M9,N11,R11:U11,Y11:AB11,AF13:AI13,AS13:AW13,AW15,BA15:BD15,BH15:BK15,BO15:BR15,BW17:BY17,CD17:CF17,CK19:CM19,CR21:CS21,CT23,CX23:DA23,DE23:DH23)</f>
+        <v>318.5</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="40" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="40" t="s">
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="40" t="s">
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="45"/>
+      <c r="X3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="41"/>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="40" t="s">
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="44"/>
+      <c r="AD3" s="45"/>
+      <c r="AE3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="AF3" s="41"/>
-      <c r="AG3" s="41"/>
-      <c r="AH3" s="41"/>
-      <c r="AI3" s="41"/>
-      <c r="AJ3" s="41"/>
-      <c r="AK3" s="42"/>
-      <c r="AL3" s="40" t="s">
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="45"/>
+      <c r="AL3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="AM3" s="41"/>
-      <c r="AN3" s="41"/>
-      <c r="AO3" s="41"/>
-      <c r="AP3" s="41"/>
-      <c r="AQ3" s="41"/>
-      <c r="AR3" s="42"/>
-      <c r="AS3" s="40" t="s">
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="44"/>
+      <c r="AO3" s="44"/>
+      <c r="AP3" s="44"/>
+      <c r="AQ3" s="44"/>
+      <c r="AR3" s="45"/>
+      <c r="AS3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AT3" s="41"/>
-      <c r="AU3" s="41"/>
-      <c r="AV3" s="41"/>
-      <c r="AW3" s="41"/>
-      <c r="AX3" s="41"/>
-      <c r="AY3" s="42"/>
-      <c r="AZ3" s="40" t="s">
+      <c r="AT3" s="44"/>
+      <c r="AU3" s="44"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="44"/>
+      <c r="AX3" s="44"/>
+      <c r="AY3" s="45"/>
+      <c r="AZ3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="BA3" s="41"/>
-      <c r="BB3" s="41"/>
-      <c r="BC3" s="41"/>
-      <c r="BD3" s="41"/>
-      <c r="BE3" s="41"/>
-      <c r="BF3" s="42"/>
-      <c r="BG3" s="40" t="s">
+      <c r="BA3" s="44"/>
+      <c r="BB3" s="44"/>
+      <c r="BC3" s="44"/>
+      <c r="BD3" s="44"/>
+      <c r="BE3" s="44"/>
+      <c r="BF3" s="45"/>
+      <c r="BG3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="BH3" s="41"/>
-      <c r="BI3" s="41"/>
-      <c r="BJ3" s="41"/>
-      <c r="BK3" s="41"/>
-      <c r="BL3" s="41"/>
-      <c r="BM3" s="42"/>
-      <c r="BN3" s="40" t="s">
+      <c r="BH3" s="44"/>
+      <c r="BI3" s="44"/>
+      <c r="BJ3" s="44"/>
+      <c r="BK3" s="44"/>
+      <c r="BL3" s="44"/>
+      <c r="BM3" s="45"/>
+      <c r="BN3" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="BO3" s="41"/>
-      <c r="BP3" s="41"/>
-      <c r="BQ3" s="41"/>
-      <c r="BR3" s="41"/>
-      <c r="BS3" s="41"/>
-      <c r="BT3" s="42"/>
-      <c r="BU3" s="40" t="s">
+      <c r="BO3" s="44"/>
+      <c r="BP3" s="44"/>
+      <c r="BQ3" s="44"/>
+      <c r="BR3" s="44"/>
+      <c r="BS3" s="44"/>
+      <c r="BT3" s="45"/>
+      <c r="BU3" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="BV3" s="41"/>
-      <c r="BW3" s="41"/>
-      <c r="BX3" s="41"/>
-      <c r="BY3" s="41"/>
-      <c r="BZ3" s="41"/>
-      <c r="CA3" s="42"/>
-      <c r="CB3" s="40" t="s">
+      <c r="BV3" s="44"/>
+      <c r="BW3" s="44"/>
+      <c r="BX3" s="44"/>
+      <c r="BY3" s="44"/>
+      <c r="BZ3" s="44"/>
+      <c r="CA3" s="45"/>
+      <c r="CB3" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="CC3" s="41"/>
-      <c r="CD3" s="41"/>
-      <c r="CE3" s="41"/>
-      <c r="CF3" s="41"/>
-      <c r="CG3" s="41"/>
-      <c r="CH3" s="42"/>
-      <c r="CI3" s="40" t="s">
+      <c r="CC3" s="44"/>
+      <c r="CD3" s="44"/>
+      <c r="CE3" s="44"/>
+      <c r="CF3" s="44"/>
+      <c r="CG3" s="44"/>
+      <c r="CH3" s="45"/>
+      <c r="CI3" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="CJ3" s="41"/>
-      <c r="CK3" s="41"/>
-      <c r="CL3" s="41"/>
-      <c r="CM3" s="41"/>
-      <c r="CN3" s="41"/>
-      <c r="CO3" s="42"/>
-      <c r="CP3" s="40" t="s">
+      <c r="CJ3" s="44"/>
+      <c r="CK3" s="44"/>
+      <c r="CL3" s="44"/>
+      <c r="CM3" s="44"/>
+      <c r="CN3" s="44"/>
+      <c r="CO3" s="45"/>
+      <c r="CP3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="CQ3" s="41"/>
-      <c r="CR3" s="41"/>
-      <c r="CS3" s="41"/>
-      <c r="CT3" s="41"/>
-      <c r="CU3" s="41"/>
-      <c r="CV3" s="42"/>
-      <c r="CW3" s="40" t="s">
+      <c r="CQ3" s="44"/>
+      <c r="CR3" s="44"/>
+      <c r="CS3" s="44"/>
+      <c r="CT3" s="44"/>
+      <c r="CU3" s="44"/>
+      <c r="CV3" s="45"/>
+      <c r="CW3" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="CX3" s="41"/>
-      <c r="CY3" s="41"/>
-      <c r="CZ3" s="41"/>
-      <c r="DA3" s="41"/>
-      <c r="DB3" s="41"/>
-      <c r="DC3" s="42"/>
-      <c r="DD3" s="40" t="s">
+      <c r="CX3" s="44"/>
+      <c r="CY3" s="44"/>
+      <c r="CZ3" s="44"/>
+      <c r="DA3" s="44"/>
+      <c r="DB3" s="44"/>
+      <c r="DC3" s="45"/>
+      <c r="DD3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="DE3" s="41"/>
-      <c r="DF3" s="41"/>
-      <c r="DG3" s="41"/>
-      <c r="DH3" s="41"/>
-      <c r="DI3" s="41"/>
-      <c r="DJ3" s="42"/>
-      <c r="DK3" s="40" t="s">
+      <c r="DE3" s="44"/>
+      <c r="DF3" s="44"/>
+      <c r="DG3" s="44"/>
+      <c r="DH3" s="44"/>
+      <c r="DI3" s="44"/>
+      <c r="DJ3" s="45"/>
+      <c r="DK3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="DL3" s="41"/>
-      <c r="DM3" s="41"/>
-      <c r="DN3" s="41"/>
-      <c r="DO3" s="41"/>
-      <c r="DP3" s="41"/>
-      <c r="DQ3" s="42"/>
-      <c r="DR3" s="40" t="s">
+      <c r="DL3" s="44"/>
+      <c r="DM3" s="44"/>
+      <c r="DN3" s="44"/>
+      <c r="DO3" s="44"/>
+      <c r="DP3" s="44"/>
+      <c r="DQ3" s="45"/>
+      <c r="DR3" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="DS3" s="41"/>
-      <c r="DT3" s="41"/>
-      <c r="DU3" s="41"/>
-      <c r="DV3" s="41"/>
-      <c r="DW3" s="41"/>
-      <c r="DX3" s="42"/>
-      <c r="DY3" s="46" t="s">
+      <c r="DS3" s="44"/>
+      <c r="DT3" s="44"/>
+      <c r="DU3" s="44"/>
+      <c r="DV3" s="44"/>
+      <c r="DW3" s="44"/>
+      <c r="DX3" s="45"/>
+      <c r="DY3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="DZ3" s="47"/>
-      <c r="EA3" s="47"/>
-      <c r="EB3" s="47"/>
-      <c r="EC3" s="47"/>
-      <c r="ED3" s="47"/>
-      <c r="EE3" s="48"/>
-      <c r="EF3" s="46" t="s">
+      <c r="DZ3" s="50"/>
+      <c r="EA3" s="50"/>
+      <c r="EB3" s="50"/>
+      <c r="EC3" s="50"/>
+      <c r="ED3" s="50"/>
+      <c r="EE3" s="51"/>
+      <c r="EF3" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="EG3" s="47"/>
-      <c r="EH3" s="47"/>
-      <c r="EI3" s="47"/>
-      <c r="EJ3" s="47"/>
-      <c r="EK3" s="47"/>
-      <c r="EL3" s="48"/>
+      <c r="EG3" s="50"/>
+      <c r="EH3" s="50"/>
+      <c r="EI3" s="50"/>
+      <c r="EJ3" s="50"/>
+      <c r="EK3" s="50"/>
+      <c r="EL3" s="51"/>
     </row>
     <row r="4" spans="1:143" ht="15" thickBot="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="10">
+        <f>SUM(D8:E8,G8,L10:N10,S12:U12)</f>
+        <v>22</v>
+      </c>
       <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
@@ -1988,7 +2016,7 @@
       <c r="EM4" s="19"/>
     </row>
     <row r="5" spans="1:143">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="52" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -2029,13 +2057,13 @@
       <c r="AI5" s="17"/>
       <c r="AJ5" s="17"/>
       <c r="AK5" s="11"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="17"/>
-      <c r="AN5" s="17"/>
-      <c r="AO5" s="17"/>
-      <c r="AP5" s="17"/>
-      <c r="AQ5" s="17"/>
-      <c r="AR5" s="11"/>
+      <c r="AL5" s="62"/>
+      <c r="AM5" s="63"/>
+      <c r="AN5" s="63"/>
+      <c r="AO5" s="63"/>
+      <c r="AP5" s="63"/>
+      <c r="AQ5" s="63"/>
+      <c r="AR5" s="64"/>
       <c r="AS5" s="16"/>
       <c r="AT5" s="17"/>
       <c r="AU5" s="17"/>
@@ -2136,7 +2164,7 @@
       <c r="EL5" s="11"/>
     </row>
     <row r="6" spans="1:143" ht="15" thickBot="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
@@ -2148,124 +2176,270 @@
       <c r="H6" s="1"/>
       <c r="I6" s="5"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
+      <c r="K6" s="22">
+        <v>2</v>
+      </c>
+      <c r="L6" s="22">
+        <v>2</v>
+      </c>
+      <c r="M6" s="22">
+        <v>2</v>
+      </c>
+      <c r="N6" s="22">
+        <v>2</v>
+      </c>
       <c r="O6" s="22"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22">
+        <v>2</v>
+      </c>
+      <c r="R6" s="22">
+        <v>2</v>
+      </c>
+      <c r="S6" s="22">
+        <v>2</v>
+      </c>
+      <c r="T6" s="22">
+        <v>2</v>
+      </c>
+      <c r="U6" s="22">
+        <v>2</v>
+      </c>
       <c r="V6" s="22"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="22">
+        <v>2</v>
+      </c>
       <c r="AC6" s="22"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="22"/>
-      <c r="AI6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AI6" s="22">
+        <v>2</v>
+      </c>
       <c r="AJ6" s="22"/>
-      <c r="AK6" s="20"/>
-      <c r="AL6" s="24"/>
-      <c r="AM6" s="22"/>
-      <c r="AN6" s="22"/>
-      <c r="AO6" s="22"/>
-      <c r="AP6" s="22"/>
-      <c r="AQ6" s="22"/>
-      <c r="AR6" s="20"/>
-      <c r="AS6" s="24"/>
-      <c r="AT6" s="22"/>
-      <c r="AU6" s="22"/>
-      <c r="AV6" s="22"/>
-      <c r="AW6" s="22"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="73"/>
+      <c r="AM6" s="73"/>
+      <c r="AN6" s="73"/>
+      <c r="AO6" s="73"/>
+      <c r="AP6" s="73"/>
+      <c r="AQ6" s="73"/>
+      <c r="AR6" s="73"/>
+      <c r="AS6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AT6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AU6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AV6" s="22">
+        <v>2</v>
+      </c>
+      <c r="AW6" s="22">
+        <v>2</v>
+      </c>
       <c r="AX6" s="22"/>
-      <c r="AY6" s="20"/>
-      <c r="AZ6" s="24"/>
-      <c r="BA6" s="22"/>
-      <c r="BB6" s="22"/>
-      <c r="BC6" s="22"/>
-      <c r="BD6" s="22"/>
+      <c r="AY6" s="22"/>
+      <c r="AZ6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BA6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BB6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BC6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BD6" s="22">
+        <v>2</v>
+      </c>
       <c r="BE6" s="22"/>
-      <c r="BF6" s="20"/>
-      <c r="BG6" s="24"/>
-      <c r="BH6" s="22"/>
-      <c r="BI6" s="22"/>
-      <c r="BJ6" s="22"/>
-      <c r="BK6" s="22"/>
+      <c r="BF6" s="22"/>
+      <c r="BG6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BH6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BI6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BJ6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BK6" s="22">
+        <v>2</v>
+      </c>
       <c r="BL6" s="22"/>
-      <c r="BM6" s="20"/>
-      <c r="BN6" s="24"/>
-      <c r="BO6" s="22"/>
-      <c r="BP6" s="22"/>
-      <c r="BQ6" s="22"/>
-      <c r="BR6" s="22"/>
+      <c r="BM6" s="22"/>
+      <c r="BN6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BO6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BP6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BQ6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BR6" s="22">
+        <v>2</v>
+      </c>
       <c r="BS6" s="22"/>
-      <c r="BT6" s="20"/>
-      <c r="BU6" s="24"/>
-      <c r="BV6" s="22"/>
-      <c r="BW6" s="22"/>
-      <c r="BX6" s="22"/>
-      <c r="BY6" s="22"/>
+      <c r="BT6" s="22"/>
+      <c r="BU6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BV6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BW6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BX6" s="22">
+        <v>2</v>
+      </c>
+      <c r="BY6" s="22">
+        <v>2</v>
+      </c>
       <c r="BZ6" s="22"/>
-      <c r="CA6" s="20"/>
-      <c r="CB6" s="24"/>
-      <c r="CC6" s="22"/>
-      <c r="CD6" s="22"/>
-      <c r="CE6" s="22"/>
-      <c r="CF6" s="22"/>
+      <c r="CA6" s="22"/>
+      <c r="CB6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CC6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CD6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CE6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CF6" s="22">
+        <v>2</v>
+      </c>
       <c r="CG6" s="22"/>
-      <c r="CH6" s="20"/>
-      <c r="CI6" s="24"/>
-      <c r="CJ6" s="22"/>
-      <c r="CK6" s="22"/>
-      <c r="CL6" s="22"/>
-      <c r="CM6" s="22"/>
+      <c r="CH6" s="22"/>
+      <c r="CI6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CJ6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CK6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CL6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CM6" s="22">
+        <v>2</v>
+      </c>
       <c r="CN6" s="22"/>
-      <c r="CO6" s="20"/>
-      <c r="CP6" s="24"/>
-      <c r="CQ6" s="22"/>
-      <c r="CR6" s="22"/>
-      <c r="CS6" s="22"/>
-      <c r="CT6" s="22"/>
+      <c r="CO6" s="22"/>
+      <c r="CP6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CQ6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CR6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CS6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CT6" s="22">
+        <v>2</v>
+      </c>
       <c r="CU6" s="22"/>
-      <c r="CV6" s="20"/>
-      <c r="CW6" s="24"/>
-      <c r="CX6" s="22"/>
-      <c r="CY6" s="22"/>
-      <c r="CZ6" s="22"/>
-      <c r="DA6" s="22"/>
+      <c r="CV6" s="22"/>
+      <c r="CW6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CX6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CY6" s="22">
+        <v>2</v>
+      </c>
+      <c r="CZ6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DA6" s="22">
+        <v>2</v>
+      </c>
       <c r="DB6" s="22"/>
-      <c r="DC6" s="20"/>
-      <c r="DD6" s="24"/>
-      <c r="DE6" s="22"/>
-      <c r="DF6" s="22"/>
-      <c r="DG6" s="22"/>
-      <c r="DH6" s="22"/>
+      <c r="DC6" s="22"/>
+      <c r="DD6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DE6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DF6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DG6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DH6" s="22">
+        <v>2</v>
+      </c>
       <c r="DI6" s="22"/>
-      <c r="DJ6" s="20"/>
-      <c r="DK6" s="24"/>
-      <c r="DL6" s="22"/>
-      <c r="DM6" s="22"/>
-      <c r="DN6" s="22"/>
-      <c r="DO6" s="22"/>
-      <c r="DP6" s="22"/>
-      <c r="DQ6" s="20"/>
-      <c r="DR6" s="24"/>
-      <c r="DS6" s="22"/>
-      <c r="DT6" s="22"/>
-      <c r="DU6" s="22"/>
-      <c r="DV6" s="22"/>
-      <c r="DW6" s="22"/>
-      <c r="DX6" s="20"/>
+      <c r="DJ6" s="22"/>
+      <c r="DK6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DL6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DM6" s="74"/>
+      <c r="DN6" s="74"/>
+      <c r="DO6" s="74"/>
+      <c r="DP6" s="74"/>
+      <c r="DQ6" s="74"/>
+      <c r="DR6" s="73"/>
+      <c r="DS6" s="73"/>
+      <c r="DT6" s="73"/>
+      <c r="DU6" s="73"/>
+      <c r="DV6" s="73"/>
+      <c r="DW6" s="22">
+        <v>2</v>
+      </c>
+      <c r="DX6" s="22">
+        <v>2</v>
+      </c>
       <c r="DY6" s="4"/>
       <c r="DZ6" s="1"/>
       <c r="EA6" s="1"/>
@@ -2282,24 +2456,24 @@
       <c r="EL6" s="5"/>
     </row>
     <row r="7" spans="1:143">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>41</v>
+      <c r="D7" s="22">
+        <v>2</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2</v>
+      </c>
+      <c r="F7" s="22">
+        <v>2</v>
+      </c>
+      <c r="G7" s="22">
+        <v>2</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="5"/>
@@ -2331,13 +2505,13 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="5"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="1"/>
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="5"/>
+      <c r="AL7" s="65"/>
+      <c r="AM7" s="61"/>
+      <c r="AN7" s="61"/>
+      <c r="AO7" s="61"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="61"/>
+      <c r="AR7" s="66"/>
       <c r="AS7" s="4"/>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
@@ -2438,16 +2612,22 @@
       <c r="EL7" s="5"/>
     </row>
     <row r="8" spans="1:143" ht="15" thickBot="1">
-      <c r="A8" s="36"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="60">
+        <v>2</v>
+      </c>
+      <c r="E8" s="60">
+        <v>1.5</v>
+      </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="60">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
       <c r="K8" s="1"/>
@@ -2477,13 +2657,13 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="5"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="1"/>
-      <c r="AN8" s="1"/>
-      <c r="AO8" s="1"/>
-      <c r="AP8" s="1"/>
-      <c r="AQ8" s="1"/>
-      <c r="AR8" s="5"/>
+      <c r="AL8" s="65"/>
+      <c r="AM8" s="61"/>
+      <c r="AN8" s="61"/>
+      <c r="AO8" s="61"/>
+      <c r="AP8" s="61"/>
+      <c r="AQ8" s="61"/>
+      <c r="AR8" s="66"/>
       <c r="AS8" s="4"/>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
@@ -2584,7 +2764,7 @@
       <c r="EL8" s="5"/>
     </row>
     <row r="9" spans="1:143">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="42" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -2598,14 +2778,14 @@
       <c r="H9" s="1"/>
       <c r="I9" s="5"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="22" t="s">
-        <v>41</v>
+      <c r="K9" s="22">
+        <v>2</v>
+      </c>
+      <c r="L9" s="22">
+        <v>2</v>
+      </c>
+      <c r="M9" s="22">
+        <v>2</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -2631,13 +2811,13 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="5"/>
-      <c r="AL9" s="4"/>
-      <c r="AM9" s="1"/>
-      <c r="AN9" s="1"/>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="5"/>
+      <c r="AL9" s="65"/>
+      <c r="AM9" s="61"/>
+      <c r="AN9" s="61"/>
+      <c r="AO9" s="61"/>
+      <c r="AP9" s="61"/>
+      <c r="AQ9" s="61"/>
+      <c r="AR9" s="66"/>
       <c r="AS9" s="4"/>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
@@ -2738,7 +2918,7 @@
       <c r="EL9" s="5"/>
     </row>
     <row r="10" spans="1:143" ht="15" thickBot="1">
-      <c r="A10" s="39"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -2751,9 +2931,15 @@
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="L10" s="60">
+        <v>3</v>
+      </c>
+      <c r="M10" s="60">
+        <v>2</v>
+      </c>
+      <c r="N10" s="60">
+        <v>2.5</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="4"/>
@@ -2777,13 +2963,13 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="5"/>
-      <c r="AL10" s="4"/>
-      <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
-      <c r="AO10" s="1"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="5"/>
+      <c r="AL10" s="65"/>
+      <c r="AM10" s="61"/>
+      <c r="AN10" s="61"/>
+      <c r="AO10" s="61"/>
+      <c r="AP10" s="61"/>
+      <c r="AQ10" s="61"/>
+      <c r="AR10" s="66"/>
       <c r="AS10" s="4"/>
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
@@ -2884,7 +3070,7 @@
       <c r="EL10" s="5"/>
     </row>
     <row r="11" spans="1:143">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -2901,38 +3087,38 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="22" t="s">
-        <v>41</v>
+      <c r="N11" s="22">
+        <v>2</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="S11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="T11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="U11" s="22" t="s">
-        <v>41</v>
+      <c r="R11" s="22">
+        <v>2</v>
+      </c>
+      <c r="S11" s="22">
+        <v>3</v>
+      </c>
+      <c r="T11" s="22">
+        <v>3</v>
+      </c>
+      <c r="U11" s="22">
+        <v>3</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="5"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB11" s="22" t="s">
-        <v>41</v>
+      <c r="Y11" s="22">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="22">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="22">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="22">
+        <v>2</v>
       </c>
       <c r="AC11" s="1"/>
       <c r="AD11" s="5"/>
@@ -2943,13 +3129,13 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="5"/>
-      <c r="AL11" s="4"/>
-      <c r="AM11" s="1"/>
-      <c r="AN11" s="1"/>
-      <c r="AO11" s="1"/>
-      <c r="AP11" s="1"/>
-      <c r="AQ11" s="1"/>
-      <c r="AR11" s="5"/>
+      <c r="AL11" s="65"/>
+      <c r="AM11" s="61"/>
+      <c r="AN11" s="61"/>
+      <c r="AO11" s="61"/>
+      <c r="AP11" s="61"/>
+      <c r="AQ11" s="61"/>
+      <c r="AR11" s="66"/>
       <c r="AS11" s="4"/>
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
@@ -3050,7 +3236,7 @@
       <c r="EL11" s="5"/>
     </row>
     <row r="12" spans="1:143" ht="15" thickBot="1">
-      <c r="A12" s="38"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -3065,22 +3251,28 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="61"/>
       <c r="O12" s="1"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
+      <c r="S12" s="60">
+        <v>3</v>
+      </c>
+      <c r="T12" s="60">
+        <v>3</v>
+      </c>
+      <c r="U12" s="60">
+        <v>3</v>
+      </c>
       <c r="V12" s="1"/>
       <c r="W12" s="5"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
+      <c r="Y12" s="61"/>
+      <c r="Z12" s="61"/>
+      <c r="AA12" s="61"/>
+      <c r="AB12" s="61"/>
+      <c r="AC12" s="61"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="1"/>
@@ -3089,13 +3281,13 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="5"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="1"/>
-      <c r="AN12" s="1"/>
-      <c r="AO12" s="1"/>
-      <c r="AP12" s="1"/>
-      <c r="AQ12" s="1"/>
-      <c r="AR12" s="5"/>
+      <c r="AL12" s="65"/>
+      <c r="AM12" s="61"/>
+      <c r="AN12" s="61"/>
+      <c r="AO12" s="61"/>
+      <c r="AP12" s="61"/>
+      <c r="AQ12" s="61"/>
+      <c r="AR12" s="66"/>
       <c r="AS12" s="4"/>
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
@@ -3196,7 +3388,7 @@
       <c r="EL12" s="5"/>
     </row>
     <row r="13" spans="1:143">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="38" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="21" t="s">
@@ -3224,54 +3416,48 @@
       <c r="V13" s="1"/>
       <c r="W13" s="5"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
+      <c r="Y13" s="61"/>
+      <c r="Z13" s="61"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="61"/>
+      <c r="AC13" s="61"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="4"/>
-      <c r="AF13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI13" s="22" t="s">
-        <v>41</v>
+      <c r="AF13" s="22">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="22">
+        <v>3</v>
+      </c>
+      <c r="AH13" s="22">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="22">
+        <v>2</v>
       </c>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="5"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AO13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ13" s="1"/>
-      <c r="AR13" s="5"/>
-      <c r="AS13" s="4"/>
-      <c r="AT13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AV13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW13" s="22" t="s">
-        <v>41</v>
+      <c r="AL13" s="65"/>
+      <c r="AM13" s="73"/>
+      <c r="AN13" s="73"/>
+      <c r="AO13" s="73"/>
+      <c r="AP13" s="73"/>
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="66"/>
+      <c r="AS13" s="23">
+        <v>2</v>
+      </c>
+      <c r="AT13" s="22">
+        <v>2</v>
+      </c>
+      <c r="AU13" s="22">
+        <v>2</v>
+      </c>
+      <c r="AV13" s="22">
+        <v>2</v>
+      </c>
+      <c r="AW13" s="22">
+        <v>2</v>
       </c>
       <c r="AX13" s="1"/>
       <c r="AY13" s="5"/>
@@ -3368,7 +3554,7 @@
       <c r="EL13" s="5"/>
     </row>
     <row r="14" spans="1:143" ht="15" thickBot="1">
-      <c r="A14" s="36"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
@@ -3407,13 +3593,13 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="5"/>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="1"/>
-      <c r="AN14" s="1"/>
-      <c r="AO14" s="1"/>
-      <c r="AP14" s="1"/>
-      <c r="AQ14" s="1"/>
-      <c r="AR14" s="5"/>
+      <c r="AL14" s="65"/>
+      <c r="AM14" s="61"/>
+      <c r="AN14" s="61"/>
+      <c r="AO14" s="61"/>
+      <c r="AP14" s="61"/>
+      <c r="AQ14" s="61"/>
+      <c r="AR14" s="66"/>
       <c r="AS14" s="4"/>
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
@@ -3514,7 +3700,7 @@
       <c r="EL14" s="5"/>
     </row>
     <row r="15" spans="1:143">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="38" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -3555,62 +3741,64 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="5"/>
-      <c r="AL15" s="4"/>
-      <c r="AM15" s="1"/>
-      <c r="AN15" s="1"/>
-      <c r="AO15" s="1"/>
-      <c r="AP15" s="1"/>
-      <c r="AQ15" s="1"/>
-      <c r="AR15" s="5"/>
+      <c r="AL15" s="65"/>
+      <c r="AM15" s="61"/>
+      <c r="AN15" s="61"/>
+      <c r="AO15" s="61"/>
+      <c r="AP15" s="61"/>
+      <c r="AQ15" s="61"/>
+      <c r="AR15" s="66"/>
       <c r="AS15" s="4"/>
       <c r="AT15" s="1"/>
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
-      <c r="AW15" s="22"/>
+      <c r="AW15" s="22">
+        <v>2</v>
+      </c>
       <c r="AX15" s="1"/>
       <c r="AY15" s="5"/>
       <c r="AZ15" s="4"/>
-      <c r="BA15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BC15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BD15" s="22" t="s">
-        <v>41</v>
+      <c r="BA15" s="22">
+        <v>2</v>
+      </c>
+      <c r="BB15" s="22">
+        <v>3</v>
+      </c>
+      <c r="BC15" s="22">
+        <v>3</v>
+      </c>
+      <c r="BD15" s="22">
+        <v>3</v>
       </c>
       <c r="BE15" s="1"/>
       <c r="BF15" s="5"/>
       <c r="BG15" s="4"/>
-      <c r="BH15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BI15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BJ15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BK15" s="22" t="s">
-        <v>41</v>
+      <c r="BH15" s="22">
+        <v>2</v>
+      </c>
+      <c r="BI15" s="22">
+        <v>3</v>
+      </c>
+      <c r="BJ15" s="22">
+        <v>3</v>
+      </c>
+      <c r="BK15" s="22">
+        <v>3</v>
       </c>
       <c r="BL15" s="1"/>
       <c r="BM15" s="5"/>
       <c r="BN15" s="4"/>
-      <c r="BO15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BP15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BQ15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BR15" s="22" t="s">
-        <v>41</v>
+      <c r="BO15" s="22">
+        <v>2</v>
+      </c>
+      <c r="BP15" s="22">
+        <v>3</v>
+      </c>
+      <c r="BQ15" s="22">
+        <v>3</v>
+      </c>
+      <c r="BR15" s="22">
+        <v>3</v>
       </c>
       <c r="BS15" s="1"/>
       <c r="BT15" s="5"/>
@@ -3686,7 +3874,7 @@
       <c r="EL15" s="5"/>
     </row>
     <row r="16" spans="1:143" ht="15" thickBot="1">
-      <c r="A16" s="36"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -3725,13 +3913,13 @@
       <c r="AI16" s="9"/>
       <c r="AJ16" s="9"/>
       <c r="AK16" s="13"/>
-      <c r="AL16" s="15"/>
-      <c r="AM16" s="9"/>
-      <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
-      <c r="AP16" s="9"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="13"/>
+      <c r="AL16" s="67"/>
+      <c r="AM16" s="68"/>
+      <c r="AN16" s="68"/>
+      <c r="AO16" s="68"/>
+      <c r="AP16" s="68"/>
+      <c r="AQ16" s="68"/>
+      <c r="AR16" s="69"/>
       <c r="AS16" s="15"/>
       <c r="AT16" s="9"/>
       <c r="AU16" s="9"/>
@@ -3832,7 +4020,7 @@
       <c r="EL16" s="13"/>
     </row>
     <row r="17" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="38" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -3873,13 +4061,13 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="5"/>
-      <c r="AL17" s="4"/>
-      <c r="AM17" s="1"/>
-      <c r="AN17" s="1"/>
-      <c r="AO17" s="1"/>
-      <c r="AP17" s="1"/>
-      <c r="AQ17" s="1"/>
-      <c r="AR17" s="5"/>
+      <c r="AL17" s="65"/>
+      <c r="AM17" s="61"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="61"/>
+      <c r="AP17" s="61"/>
+      <c r="AQ17" s="61"/>
+      <c r="AR17" s="66"/>
       <c r="AS17" s="4"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
@@ -3909,32 +4097,28 @@
       <c r="BS17" s="1"/>
       <c r="BT17" s="5"/>
       <c r="BU17" s="4"/>
-      <c r="BV17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BW17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BX17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="BY17" s="22" t="s">
-        <v>41</v>
+      <c r="BV17" s="1"/>
+      <c r="BW17" s="22">
+        <v>2</v>
+      </c>
+      <c r="BX17" s="22">
+        <v>2</v>
+      </c>
+      <c r="BY17" s="22">
+        <v>2</v>
       </c>
       <c r="BZ17" s="1"/>
       <c r="CA17" s="5"/>
       <c r="CB17" s="4"/>
-      <c r="CC17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CD17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CE17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CF17" s="22" t="s">
-        <v>41</v>
+      <c r="CC17" s="1"/>
+      <c r="CD17" s="22">
+        <v>2</v>
+      </c>
+      <c r="CE17" s="22">
+        <v>2</v>
+      </c>
+      <c r="CF17" s="22">
+        <v>2</v>
       </c>
       <c r="CG17" s="1"/>
       <c r="CH17" s="5"/>
@@ -3996,7 +4180,7 @@
       <c r="EL17" s="5"/>
     </row>
     <row r="18" spans="1:142" ht="15" thickBot="1">
-      <c r="A18" s="36"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
@@ -4035,13 +4219,13 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="5"/>
-      <c r="AL18" s="4"/>
-      <c r="AM18" s="1"/>
-      <c r="AN18" s="1"/>
-      <c r="AO18" s="1"/>
-      <c r="AP18" s="1"/>
-      <c r="AQ18" s="1"/>
-      <c r="AR18" s="5"/>
+      <c r="AL18" s="65"/>
+      <c r="AM18" s="61"/>
+      <c r="AN18" s="61"/>
+      <c r="AO18" s="61"/>
+      <c r="AP18" s="61"/>
+      <c r="AQ18" s="61"/>
+      <c r="AR18" s="66"/>
       <c r="AS18" s="4"/>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
@@ -4142,7 +4326,7 @@
       <c r="EL18" s="5"/>
     </row>
     <row r="19" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="46" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -4183,13 +4367,13 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="5"/>
-      <c r="AL19" s="4"/>
-      <c r="AM19" s="1"/>
-      <c r="AN19" s="1"/>
-      <c r="AO19" s="1"/>
-      <c r="AP19" s="1"/>
-      <c r="AQ19" s="1"/>
-      <c r="AR19" s="5"/>
+      <c r="AL19" s="65"/>
+      <c r="AM19" s="61"/>
+      <c r="AN19" s="61"/>
+      <c r="AO19" s="61"/>
+      <c r="AP19" s="61"/>
+      <c r="AQ19" s="61"/>
+      <c r="AR19" s="66"/>
       <c r="AS19" s="4"/>
       <c r="AT19" s="1"/>
       <c r="AU19" s="1"/>
@@ -4234,14 +4418,14 @@
       <c r="CH19" s="5"/>
       <c r="CI19" s="4"/>
       <c r="CJ19" s="1"/>
-      <c r="CK19" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CL19" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CM19" s="22" t="s">
-        <v>41</v>
+      <c r="CK19" s="22">
+        <v>2</v>
+      </c>
+      <c r="CL19" s="22">
+        <v>2</v>
+      </c>
+      <c r="CM19" s="22">
+        <v>2</v>
       </c>
       <c r="CN19" s="1"/>
       <c r="CO19" s="5"/>
@@ -4296,7 +4480,7 @@
       <c r="EL19" s="5"/>
     </row>
     <row r="20" spans="1:142" ht="15" thickBot="1">
-      <c r="A20" s="45"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -4335,13 +4519,13 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="5"/>
-      <c r="AL20" s="4"/>
-      <c r="AM20" s="1"/>
-      <c r="AN20" s="1"/>
-      <c r="AO20" s="1"/>
-      <c r="AP20" s="1"/>
-      <c r="AQ20" s="1"/>
-      <c r="AR20" s="5"/>
+      <c r="AL20" s="65"/>
+      <c r="AM20" s="61"/>
+      <c r="AN20" s="61"/>
+      <c r="AO20" s="61"/>
+      <c r="AP20" s="61"/>
+      <c r="AQ20" s="61"/>
+      <c r="AR20" s="66"/>
       <c r="AS20" s="4"/>
       <c r="AT20" s="1"/>
       <c r="AU20" s="1"/>
@@ -4442,7 +4626,7 @@
       <c r="EL20" s="5"/>
     </row>
     <row r="21" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="46" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="21" t="s">
@@ -4483,13 +4667,13 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="5"/>
-      <c r="AL21" s="4"/>
-      <c r="AM21" s="1"/>
-      <c r="AN21" s="1"/>
-      <c r="AO21" s="1"/>
-      <c r="AP21" s="1"/>
-      <c r="AQ21" s="1"/>
-      <c r="AR21" s="5"/>
+      <c r="AL21" s="65"/>
+      <c r="AM21" s="61"/>
+      <c r="AN21" s="61"/>
+      <c r="AO21" s="61"/>
+      <c r="AP21" s="61"/>
+      <c r="AQ21" s="61"/>
+      <c r="AR21" s="66"/>
       <c r="AS21" s="4"/>
       <c r="AT21" s="1"/>
       <c r="AU21" s="1"/>
@@ -4541,15 +4725,13 @@
       <c r="CO21" s="5"/>
       <c r="CP21" s="4"/>
       <c r="CQ21" s="1"/>
-      <c r="CR21" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CS21" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CT21" s="22" t="s">
-        <v>41</v>
-      </c>
+      <c r="CR21" s="22">
+        <v>2</v>
+      </c>
+      <c r="CS21" s="22">
+        <v>2</v>
+      </c>
+      <c r="CT21" s="1"/>
       <c r="CU21" s="1"/>
       <c r="CV21" s="5"/>
       <c r="CW21" s="4"/>
@@ -4596,7 +4778,7 @@
       <c r="EL21" s="5"/>
     </row>
     <row r="22" spans="1:142" ht="15" thickBot="1">
-      <c r="A22" s="45"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
@@ -4635,13 +4817,13 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="5"/>
-      <c r="AL22" s="4"/>
-      <c r="AM22" s="1"/>
-      <c r="AN22" s="1"/>
-      <c r="AO22" s="1"/>
-      <c r="AP22" s="1"/>
-      <c r="AQ22" s="1"/>
-      <c r="AR22" s="5"/>
+      <c r="AL22" s="65"/>
+      <c r="AM22" s="61"/>
+      <c r="AN22" s="61"/>
+      <c r="AO22" s="61"/>
+      <c r="AP22" s="61"/>
+      <c r="AQ22" s="61"/>
+      <c r="AR22" s="66"/>
       <c r="AS22" s="4"/>
       <c r="AT22" s="1"/>
       <c r="AU22" s="1"/>
@@ -4695,7 +4877,6 @@
       <c r="CQ22" s="1"/>
       <c r="CR22" s="1"/>
       <c r="CS22" s="1"/>
-      <c r="CT22" s="1"/>
       <c r="CU22" s="1"/>
       <c r="CV22" s="5"/>
       <c r="CW22" s="4"/>
@@ -4742,7 +4923,7 @@
       <c r="EL22" s="5"/>
     </row>
     <row r="23" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -4783,13 +4964,13 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="5"/>
-      <c r="AL23" s="4"/>
-      <c r="AM23" s="1"/>
-      <c r="AN23" s="1"/>
-      <c r="AO23" s="1"/>
-      <c r="AP23" s="1"/>
-      <c r="AQ23" s="1"/>
-      <c r="AR23" s="5"/>
+      <c r="AL23" s="65"/>
+      <c r="AM23" s="61"/>
+      <c r="AN23" s="61"/>
+      <c r="AO23" s="61"/>
+      <c r="AP23" s="61"/>
+      <c r="AQ23" s="61"/>
+      <c r="AR23" s="66"/>
       <c r="AS23" s="4"/>
       <c r="AT23" s="1"/>
       <c r="AU23" s="1"/>
@@ -4843,73 +5024,63 @@
       <c r="CQ23" s="1"/>
       <c r="CR23" s="1"/>
       <c r="CS23" s="1"/>
-      <c r="CT23" s="1"/>
+      <c r="CT23" s="22">
+        <v>2</v>
+      </c>
       <c r="CU23" s="1"/>
       <c r="CV23" s="5"/>
       <c r="CW23" s="4"/>
-      <c r="CX23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CY23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="CZ23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DA23" s="22" t="s">
-        <v>41</v>
+      <c r="CX23" s="22">
+        <v>2</v>
+      </c>
+      <c r="CY23" s="22">
+        <v>4</v>
+      </c>
+      <c r="CZ23" s="22">
+        <v>4</v>
+      </c>
+      <c r="DA23" s="22">
+        <v>3</v>
       </c>
       <c r="DB23" s="1"/>
       <c r="DC23" s="5"/>
       <c r="DD23" s="4"/>
-      <c r="DE23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DF23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DG23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DH23" s="22" t="s">
-        <v>41</v>
+      <c r="DE23" s="22">
+        <v>2</v>
+      </c>
+      <c r="DF23" s="22">
+        <v>3</v>
+      </c>
+      <c r="DG23" s="22">
+        <v>4</v>
+      </c>
+      <c r="DH23" s="22">
+        <v>3</v>
       </c>
       <c r="DI23" s="1"/>
       <c r="DJ23" s="5"/>
       <c r="DK23" s="4"/>
-      <c r="DL23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DM23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DN23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DO23" s="22" t="s">
-        <v>41</v>
-      </c>
+      <c r="DL23" s="73"/>
+      <c r="DM23" s="73"/>
+      <c r="DN23" s="73"/>
+      <c r="DO23" s="73"/>
       <c r="DP23" s="1"/>
       <c r="DQ23" s="5"/>
       <c r="DR23" s="4"/>
-      <c r="DS23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DT23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DU23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="DV23" s="22" t="s">
-        <v>41</v>
-      </c>
+      <c r="DS23" s="73"/>
+      <c r="DT23" s="73"/>
+      <c r="DU23" s="73"/>
+      <c r="DV23" s="73"/>
       <c r="DW23" s="1"/>
       <c r="DX23" s="5"/>
-      <c r="DY23" s="4"/>
-      <c r="DZ23" s="1"/>
-      <c r="EA23" s="1"/>
-      <c r="EB23" s="1"/>
+      <c r="DY23" s="65"/>
+      <c r="DZ23" s="61"/>
+      <c r="EA23" s="22">
+        <v>5</v>
+      </c>
+      <c r="EB23" s="22">
+        <v>5</v>
+      </c>
       <c r="EC23" s="1"/>
       <c r="ED23" s="1"/>
       <c r="EE23" s="5"/>
@@ -4922,7 +5093,7 @@
       <c r="EL23" s="5"/>
     </row>
     <row r="24" spans="1:142" ht="15" thickBot="1">
-      <c r="A24" s="45"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
@@ -4961,13 +5132,13 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="5"/>
-      <c r="AL24" s="4"/>
-      <c r="AM24" s="1"/>
-      <c r="AN24" s="1"/>
-      <c r="AO24" s="1"/>
-      <c r="AP24" s="1"/>
-      <c r="AQ24" s="1"/>
-      <c r="AR24" s="5"/>
+      <c r="AL24" s="65"/>
+      <c r="AM24" s="61"/>
+      <c r="AN24" s="61"/>
+      <c r="AO24" s="61"/>
+      <c r="AP24" s="61"/>
+      <c r="AQ24" s="61"/>
+      <c r="AR24" s="66"/>
       <c r="AS24" s="4"/>
       <c r="AT24" s="1"/>
       <c r="AU24" s="1"/>
@@ -5068,7 +5239,7 @@
       <c r="EL24" s="5"/>
     </row>
     <row r="25" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="21" t="s">
@@ -5109,13 +5280,13 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="5"/>
-      <c r="AL25" s="4"/>
-      <c r="AM25" s="1"/>
-      <c r="AN25" s="1"/>
-      <c r="AO25" s="1"/>
-      <c r="AP25" s="1"/>
-      <c r="AQ25" s="1"/>
-      <c r="AR25" s="5"/>
+      <c r="AL25" s="65"/>
+      <c r="AM25" s="61"/>
+      <c r="AN25" s="61"/>
+      <c r="AO25" s="61"/>
+      <c r="AP25" s="61"/>
+      <c r="AQ25" s="61"/>
+      <c r="AR25" s="66"/>
       <c r="AS25" s="4"/>
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
@@ -5200,29 +5371,29 @@
       <c r="DV25" s="1"/>
       <c r="DW25" s="1"/>
       <c r="DX25" s="5"/>
-      <c r="DY25" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="DZ25" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="EA25" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="EB25" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="EC25" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="ED25" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="EE25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="EF25" s="24" t="s">
-        <v>41</v>
+      <c r="DY25" s="23">
+        <v>3</v>
+      </c>
+      <c r="DZ25" s="22">
+        <v>2</v>
+      </c>
+      <c r="EA25" s="22">
+        <v>3</v>
+      </c>
+      <c r="EB25" s="22">
+        <v>3</v>
+      </c>
+      <c r="EC25" s="22">
+        <v>3</v>
+      </c>
+      <c r="ED25" s="22">
+        <v>3</v>
+      </c>
+      <c r="EE25" s="20">
+        <v>3</v>
+      </c>
+      <c r="EF25" s="23">
+        <v>3</v>
       </c>
       <c r="EG25" s="1"/>
       <c r="EH25" s="1"/>
@@ -5232,7 +5403,7 @@
       <c r="EL25" s="5"/>
     </row>
     <row r="26" spans="1:142" ht="15" thickBot="1">
-      <c r="A26" s="45"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
@@ -5244,7 +5415,9 @@
       <c r="H26" s="1"/>
       <c r="I26" s="5"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -5271,13 +5444,13 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="5"/>
-      <c r="AL26" s="4"/>
-      <c r="AM26" s="1"/>
-      <c r="AN26" s="1"/>
-      <c r="AO26" s="1"/>
-      <c r="AP26" s="1"/>
-      <c r="AQ26" s="1"/>
-      <c r="AR26" s="5"/>
+      <c r="AL26" s="65"/>
+      <c r="AM26" s="61"/>
+      <c r="AN26" s="61"/>
+      <c r="AO26" s="61"/>
+      <c r="AP26" s="61"/>
+      <c r="AQ26" s="61"/>
+      <c r="AR26" s="66"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
@@ -5378,7 +5551,7 @@
       <c r="EL26" s="5"/>
     </row>
     <row r="27" spans="1:142" ht="15" customHeight="1">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="46" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -5419,13 +5592,13 @@
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="5"/>
-      <c r="AL27" s="4"/>
-      <c r="AM27" s="1"/>
-      <c r="AN27" s="1"/>
-      <c r="AO27" s="1"/>
-      <c r="AP27" s="1"/>
-      <c r="AQ27" s="1"/>
-      <c r="AR27" s="5"/>
+      <c r="AL27" s="65"/>
+      <c r="AM27" s="61"/>
+      <c r="AN27" s="61"/>
+      <c r="AO27" s="61"/>
+      <c r="AP27" s="61"/>
+      <c r="AQ27" s="61"/>
+      <c r="AR27" s="66"/>
       <c r="AS27" s="4"/>
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
@@ -5518,8 +5691,8 @@
       <c r="ED27" s="17"/>
       <c r="EE27" s="11"/>
       <c r="EF27" s="16"/>
-      <c r="EG27" s="25" t="s">
-        <v>42</v>
+      <c r="EG27" s="24">
+        <v>0.5</v>
       </c>
       <c r="EH27" s="17"/>
       <c r="EI27" s="17"/>
@@ -5528,7 +5701,7 @@
       <c r="EL27" s="11"/>
     </row>
     <row r="28" spans="1:142" ht="15" thickBot="1">
-      <c r="A28" s="44"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="8" t="s">
         <v>32</v>
       </c>
@@ -5567,13 +5740,13 @@
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
       <c r="AK28" s="8"/>
-      <c r="AL28" s="6"/>
-      <c r="AM28" s="7"/>
-      <c r="AN28" s="7"/>
-      <c r="AO28" s="7"/>
-      <c r="AP28" s="7"/>
-      <c r="AQ28" s="7"/>
-      <c r="AR28" s="8"/>
+      <c r="AL28" s="70"/>
+      <c r="AM28" s="71"/>
+      <c r="AN28" s="71"/>
+      <c r="AO28" s="71"/>
+      <c r="AP28" s="71"/>
+      <c r="AQ28" s="71"/>
+      <c r="AR28" s="72"/>
       <c r="AS28" s="6"/>
       <c r="AT28" s="7"/>
       <c r="AU28" s="7"/>
@@ -5719,7 +5892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FF6EFD-F608-4DA6-AB00-E35874012156}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="79" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="72" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -5729,473 +5902,473 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="26" t="s">
+      <c r="C3" s="53"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B4" s="57">
+        <v>1</v>
+      </c>
+      <c r="C4" s="57"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="50"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="26" t="s">
+      <c r="B5" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="54">
-        <v>1</v>
-      </c>
-      <c r="C4" s="54"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="26" t="s">
+      <c r="C5" s="53"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B6" s="58">
+        <v>45524</v>
+      </c>
+      <c r="C6" s="58"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="50"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="26" t="s">
+      <c r="B7" s="59">
+        <v>45671</v>
+      </c>
+      <c r="C7" s="59"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="55">
-        <v>45524</v>
-      </c>
-      <c r="C6" s="55"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="26" t="s">
+      <c r="B8" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="56">
-        <v>45671</v>
-      </c>
-      <c r="C7" s="56"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="50"/>
+      <c r="C8" s="53"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="54"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="51"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="52" t="s">
+      <c r="B15" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="27" t="s">
+      <c r="C15" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="28" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="28">
+        <v>1</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="28" t="s">
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="29">
+        <v>2</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="28">
+        <v>3</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29">
+      <c r="A19" s="35">
+        <v>4</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="28">
+        <v>5</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="29">
+        <v>6</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="28">
+        <v>7</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="29">
+        <v>8</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="28">
+        <v>9</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="29">
+        <v>10</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="28">
+        <v>11</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="29">
+        <v>12</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="29">
+      <c r="A28" s="33">
+        <v>13</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29">
+      <c r="A29" s="35">
+        <v>14</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="28">
+        <v>15</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="29">
+        <v>16</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="28">
+        <v>17</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="29">
+        <v>18</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="28">
+        <v>19</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="29">
+        <v>20</v>
+      </c>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="28">
+        <v>21</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="29">
+        <v>22</v>
+      </c>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="55" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="29">
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="28">
         <v>1</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B45" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="29">
+        <v>2</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="28">
+        <v>3</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="29">
+        <v>4</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="28">
+        <v>5</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="29">
+        <v>6</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="28">
+        <v>7</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="29">
+        <v>8</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="28">
+        <v>9</v>
+      </c>
+      <c r="B53" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="30">
-        <v>2</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="29">
-        <v>3</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="29">
-      <c r="A19" s="61">
-        <v>4</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="29">
-        <v>5</v>
-      </c>
-      <c r="B20" s="59" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="30">
-        <v>6</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="29">
-        <v>7</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="30">
-        <v>8</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="29">
-        <v>9</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="30">
+      <c r="C53" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="29">
         <v>10</v>
       </c>
-      <c r="B25" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="29">
+      <c r="B54" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="28">
         <v>11</v>
       </c>
-      <c r="B26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="30">
-        <v>12</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="29">
-      <c r="A28" s="58">
-        <v>13</v>
-      </c>
-      <c r="B28" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="58" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="29">
-      <c r="A29" s="61">
-        <v>14</v>
-      </c>
-      <c r="B29" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="29">
-        <v>15</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="30">
-        <v>16</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="29">
-        <v>17</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="30">
-        <v>18</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="29">
-        <v>19</v>
-      </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="30">
-        <v>20</v>
-      </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="29">
-        <v>21</v>
-      </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="30">
-        <v>22</v>
-      </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="28" t="s">
+      <c r="B55" s="28"/>
+      <c r="C55" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="29">
-        <v>1</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="30">
-        <v>2</v>
-      </c>
-      <c r="B46" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="29">
-        <v>3</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="30">
-        <v>4</v>
-      </c>
-      <c r="B48" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="29">
-        <v>5</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="30">
-        <v>6</v>
-      </c>
-      <c r="B50" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="29">
-        <v>7</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="30">
-        <v>8</v>
-      </c>
-      <c r="B52" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="29">
-        <v>9</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="30">
-        <v>10</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="29">
-        <v>11</v>
-      </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
added Themenwahl as Word and Pdf datei and changed some Requirements
</commit_message>
<xml_diff>
--- a/Zeitplan_Anforderungen/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
+++ b/Zeitplan_Anforderungen/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4b8c2adf92642a/Berufsschule/BuP/5_Semester/Marvin/Zeitplan_Anforderungen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="433" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F603C4F-5F6E-40F3-A67A-5376AC307DCF}"/>
+  <xr:revisionPtr revIDLastSave="444" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CCDB860-451A-458D-BE60-3AEC287423AF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="1" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <t>Das ich den Sensor Print an eine der Seiten des Türrahmens montieren kann (Wenn Lichtschranke)</t>
   </si>
   <si>
-    <t>Dass Batterie nicht wircklich sichtbar ist</t>
-  </si>
-  <si>
     <t>Das die Gehäuse so klein wie möglich sind</t>
   </si>
   <si>
@@ -334,15 +331,9 @@
     <t>Auf der Platine des Sensors ein Kleines Motiv von Marvin ist (aus Hitchhickers guide to the galaxy)</t>
   </si>
   <si>
-    <t>Die audio anlage soll mit einem Sensor ausgestattet sein, der bei annäherung oder Durchquerung aktiviert wird (Infrarot  oder Lichtschranken)</t>
-  </si>
-  <si>
     <t>Der Sensor soll selbst aufgenommene Audiosignale auslösen</t>
   </si>
   <si>
-    <t>Es sollen audiodateien in verschiedenen Formaten abgespielt werden können (MP3, WAV)</t>
-  </si>
-  <si>
     <t>Jede Aktivierung des Sensors soll nur eine Audiodatei abspielen.</t>
   </si>
   <si>
@@ -355,18 +346,9 @@
     <t>Die Lautstärke soll physisch eingestellt werden können (Regler oder Tasten)</t>
   </si>
   <si>
-    <t>Eine LED soll anzeigen ob der Sensor ein Signal gegeben hat.</t>
-  </si>
-  <si>
     <t>Die Lautstärke soll nach dem Ausschalten der Anlage gespeichert werden</t>
   </si>
   <si>
-    <t>Am Output des Audio Prints sollen 50db ±10db heraus gegeben werden.</t>
-  </si>
-  <si>
-    <t>Am Input des Audio Prints soll ich nicht mehr als 3.3V haben.</t>
-  </si>
-  <si>
     <t>Der Sensor soll nach 0,5 Sekunder nach Annäherung oder Durchquerung reagieren.</t>
   </si>
   <si>
@@ -385,9 +367,6 @@
     <t>Es soll eine Zeitschalterfunktion geben, mit der due Anlage zu einer bestimmten Uhrzeit aktiviert wird.</t>
   </si>
   <si>
-    <t>Es sollen verschiedene Wiedergabeodi geben</t>
-  </si>
-  <si>
     <t>1. Einzelwiedergabe: wird nur eine datei abgespielt</t>
   </si>
   <si>
@@ -401,6 +380,27 @@
   </si>
   <si>
     <t>pwd</t>
+  </si>
+  <si>
+    <t>Am Input des Audio Prints soll ich nicht mehr als 3.3V haben. (AC oder DC)</t>
+  </si>
+  <si>
+    <t>Am Output des Audio Prints sollen 50dB ±10dB heraus gegeben werden. (dBu?)</t>
+  </si>
+  <si>
+    <t>Eine LED soll anzeigen ob der Bewegungssensor eine Bewegung detektiert hat.</t>
+  </si>
+  <si>
+    <t>Die Audioanlage soll mit einem Sensor ausgestattet sein, der bei Annäherung oder Durchquerung aktiviert wird.</t>
+  </si>
+  <si>
+    <t>Es sollen Audiodateien in verschiedenen Formaten abgespielt werden können (MP3, WAV)</t>
+  </si>
+  <si>
+    <t>Es sollen verschiedene Wiedergabemodi geben</t>
+  </si>
+  <si>
+    <t>Dass Batterie nicht wirklich sichtbar ist</t>
   </si>
 </sst>
 </file>
@@ -900,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -947,25 +947,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -977,6 +973,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -986,16 +988,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1019,21 +1021,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1055,10 +1042,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1380,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8C9801-39B9-4B26-94D0-9F2F7C9746D6}">
   <dimension ref="A1:EM28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="49" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="49" workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -1390,15 +1373,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:143" ht="18.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="52"/>
     </row>
     <row r="2" spans="1:143" ht="15" thickBot="1"/>
     <row r="3" spans="1:143" ht="15" thickBot="1">
       <c r="A3" s="22" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2">
         <f>SUM(EG27,DY25:EF25,EA23:EB23,K6:DX6,D7:G7,K9:M9,N11,R11:U11,Y11:AB11,AF13:AI13,AS13:AW13,AW15,BA15:BD15,BH15:BK15,BO15:BR15,BW17:BY17,CD17:CF17,CK19:CM19,CR21:CS21,CT23,CX23:DA23,DE23:DH23)</f>
@@ -1566,28 +1549,28 @@
       <c r="DV3" s="44"/>
       <c r="DW3" s="44"/>
       <c r="DX3" s="45"/>
-      <c r="DY3" s="49" t="s">
+      <c r="DY3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="DZ3" s="50"/>
-      <c r="EA3" s="50"/>
-      <c r="EB3" s="50"/>
-      <c r="EC3" s="50"/>
-      <c r="ED3" s="50"/>
-      <c r="EE3" s="51"/>
-      <c r="EF3" s="49" t="s">
+      <c r="DZ3" s="39"/>
+      <c r="EA3" s="39"/>
+      <c r="EB3" s="39"/>
+      <c r="EC3" s="39"/>
+      <c r="ED3" s="39"/>
+      <c r="EE3" s="40"/>
+      <c r="EF3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="EG3" s="50"/>
-      <c r="EH3" s="50"/>
-      <c r="EI3" s="50"/>
-      <c r="EJ3" s="50"/>
-      <c r="EK3" s="50"/>
-      <c r="EL3" s="51"/>
+      <c r="EG3" s="39"/>
+      <c r="EH3" s="39"/>
+      <c r="EI3" s="39"/>
+      <c r="EJ3" s="39"/>
+      <c r="EK3" s="39"/>
+      <c r="EL3" s="40"/>
     </row>
     <row r="4" spans="1:143" ht="15" thickBot="1">
-      <c r="A4" s="60" t="s">
-        <v>87</v>
+      <c r="A4" s="36" t="s">
+        <v>80</v>
       </c>
       <c r="B4" s="10">
         <f>SUM(D8:E8,G8,L10:N10,S12:U12)</f>
@@ -2016,7 +1999,7 @@
       <c r="EM4" s="19"/>
     </row>
     <row r="5" spans="1:143">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="46" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -2057,13 +2040,13 @@
       <c r="AI5" s="17"/>
       <c r="AJ5" s="17"/>
       <c r="AK5" s="11"/>
-      <c r="AL5" s="62"/>
-      <c r="AM5" s="63"/>
-      <c r="AN5" s="63"/>
-      <c r="AO5" s="63"/>
-      <c r="AP5" s="63"/>
-      <c r="AQ5" s="63"/>
-      <c r="AR5" s="64"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="17"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="17"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="11"/>
       <c r="AS5" s="16"/>
       <c r="AT5" s="17"/>
       <c r="AU5" s="17"/>
@@ -2164,7 +2147,7 @@
       <c r="EL5" s="11"/>
     </row>
     <row r="6" spans="1:143" ht="15" thickBot="1">
-      <c r="A6" s="42"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
@@ -2241,13 +2224,13 @@
       </c>
       <c r="AJ6" s="22"/>
       <c r="AK6" s="22"/>
-      <c r="AL6" s="73"/>
-      <c r="AM6" s="73"/>
-      <c r="AN6" s="73"/>
-      <c r="AO6" s="73"/>
-      <c r="AP6" s="73"/>
-      <c r="AQ6" s="73"/>
-      <c r="AR6" s="73"/>
+      <c r="AL6" s="37"/>
+      <c r="AM6" s="37"/>
+      <c r="AN6" s="37"/>
+      <c r="AO6" s="37"/>
+      <c r="AP6" s="37"/>
+      <c r="AQ6" s="37"/>
+      <c r="AR6" s="37"/>
       <c r="AS6" s="22">
         <v>2</v>
       </c>
@@ -2424,16 +2407,16 @@
       <c r="DL6" s="22">
         <v>2</v>
       </c>
-      <c r="DM6" s="74"/>
-      <c r="DN6" s="74"/>
-      <c r="DO6" s="74"/>
-      <c r="DP6" s="74"/>
-      <c r="DQ6" s="74"/>
-      <c r="DR6" s="73"/>
-      <c r="DS6" s="73"/>
-      <c r="DT6" s="73"/>
-      <c r="DU6" s="73"/>
-      <c r="DV6" s="73"/>
+      <c r="DM6" s="37"/>
+      <c r="DN6" s="37"/>
+      <c r="DO6" s="37"/>
+      <c r="DP6" s="37"/>
+      <c r="DQ6" s="37"/>
+      <c r="DR6" s="37"/>
+      <c r="DS6" s="37"/>
+      <c r="DT6" s="37"/>
+      <c r="DU6" s="37"/>
+      <c r="DV6" s="37"/>
       <c r="DW6" s="22">
         <v>2</v>
       </c>
@@ -2456,7 +2439,7 @@
       <c r="EL6" s="5"/>
     </row>
     <row r="7" spans="1:143">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -2505,13 +2488,13 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="5"/>
-      <c r="AL7" s="65"/>
-      <c r="AM7" s="61"/>
-      <c r="AN7" s="61"/>
-      <c r="AO7" s="61"/>
-      <c r="AP7" s="61"/>
-      <c r="AQ7" s="61"/>
-      <c r="AR7" s="66"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="5"/>
       <c r="AS7" s="4"/>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
@@ -2612,19 +2595,19 @@
       <c r="EL7" s="5"/>
     </row>
     <row r="8" spans="1:143" ht="15" thickBot="1">
-      <c r="A8" s="39"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="60">
-        <v>2</v>
-      </c>
-      <c r="E8" s="60">
+      <c r="D8" s="36">
+        <v>2</v>
+      </c>
+      <c r="E8" s="36">
         <v>1.5</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="60">
+      <c r="G8" s="36">
         <v>2</v>
       </c>
       <c r="H8" s="1"/>
@@ -2657,13 +2640,13 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="5"/>
-      <c r="AL8" s="65"/>
-      <c r="AM8" s="61"/>
-      <c r="AN8" s="61"/>
-      <c r="AO8" s="61"/>
-      <c r="AP8" s="61"/>
-      <c r="AQ8" s="61"/>
-      <c r="AR8" s="66"/>
+      <c r="AL8" s="4"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="5"/>
       <c r="AS8" s="4"/>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
@@ -2764,7 +2747,7 @@
       <c r="EL8" s="5"/>
     </row>
     <row r="9" spans="1:143">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="47" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -2811,13 +2794,13 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="5"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="61"/>
-      <c r="AN9" s="61"/>
-      <c r="AO9" s="61"/>
-      <c r="AP9" s="61"/>
-      <c r="AQ9" s="61"/>
-      <c r="AR9" s="66"/>
+      <c r="AL9" s="4"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="5"/>
       <c r="AS9" s="4"/>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
@@ -2918,7 +2901,7 @@
       <c r="EL9" s="5"/>
     </row>
     <row r="10" spans="1:143" ht="15" thickBot="1">
-      <c r="A10" s="42"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -2931,13 +2914,13 @@
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="60">
+      <c r="L10" s="36">
         <v>3</v>
       </c>
-      <c r="M10" s="60">
-        <v>2</v>
-      </c>
-      <c r="N10" s="60">
+      <c r="M10" s="36">
+        <v>2</v>
+      </c>
+      <c r="N10" s="36">
         <v>2.5</v>
       </c>
       <c r="O10" s="1"/>
@@ -2963,13 +2946,13 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="5"/>
-      <c r="AL10" s="65"/>
-      <c r="AM10" s="61"/>
-      <c r="AN10" s="61"/>
-      <c r="AO10" s="61"/>
-      <c r="AP10" s="61"/>
-      <c r="AQ10" s="61"/>
-      <c r="AR10" s="66"/>
+      <c r="AL10" s="4"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="5"/>
       <c r="AS10" s="4"/>
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
@@ -3070,7 +3053,7 @@
       <c r="EL10" s="5"/>
     </row>
     <row r="11" spans="1:143">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="53" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -3129,13 +3112,13 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="5"/>
-      <c r="AL11" s="65"/>
-      <c r="AM11" s="61"/>
-      <c r="AN11" s="61"/>
-      <c r="AO11" s="61"/>
-      <c r="AP11" s="61"/>
-      <c r="AQ11" s="61"/>
-      <c r="AR11" s="66"/>
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="5"/>
       <c r="AS11" s="4"/>
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
@@ -3236,7 +3219,7 @@
       <c r="EL11" s="5"/>
     </row>
     <row r="12" spans="1:143" ht="15" thickBot="1">
-      <c r="A12" s="41"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -3251,28 +3234,28 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="61"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="60">
+      <c r="S12" s="36">
         <v>3</v>
       </c>
-      <c r="T12" s="60">
+      <c r="T12" s="36">
         <v>3</v>
       </c>
-      <c r="U12" s="60">
+      <c r="U12" s="36">
         <v>3</v>
       </c>
       <c r="V12" s="1"/>
       <c r="W12" s="5"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="61"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="1"/>
@@ -3281,13 +3264,13 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="5"/>
-      <c r="AL12" s="65"/>
-      <c r="AM12" s="61"/>
-      <c r="AN12" s="61"/>
-      <c r="AO12" s="61"/>
-      <c r="AP12" s="61"/>
-      <c r="AQ12" s="61"/>
-      <c r="AR12" s="66"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="5"/>
       <c r="AS12" s="4"/>
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
@@ -3388,7 +3371,7 @@
       <c r="EL12" s="5"/>
     </row>
     <row r="13" spans="1:143">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="21" t="s">
@@ -3416,11 +3399,11 @@
       <c r="V13" s="1"/>
       <c r="W13" s="5"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="61"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="22">
@@ -3437,13 +3420,13 @@
       </c>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="5"/>
-      <c r="AL13" s="65"/>
-      <c r="AM13" s="73"/>
-      <c r="AN13" s="73"/>
-      <c r="AO13" s="73"/>
-      <c r="AP13" s="73"/>
-      <c r="AQ13" s="61"/>
-      <c r="AR13" s="66"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="37"/>
+      <c r="AN13" s="37"/>
+      <c r="AO13" s="37"/>
+      <c r="AP13" s="37"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="5"/>
       <c r="AS13" s="23">
         <v>2</v>
       </c>
@@ -3554,7 +3537,7 @@
       <c r="EL13" s="5"/>
     </row>
     <row r="14" spans="1:143" ht="15" thickBot="1">
-      <c r="A14" s="39"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
@@ -3593,13 +3576,13 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="5"/>
-      <c r="AL14" s="65"/>
-      <c r="AM14" s="61"/>
-      <c r="AN14" s="61"/>
-      <c r="AO14" s="61"/>
-      <c r="AP14" s="61"/>
-      <c r="AQ14" s="61"/>
-      <c r="AR14" s="66"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="5"/>
       <c r="AS14" s="4"/>
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
@@ -3700,7 +3683,7 @@
       <c r="EL14" s="5"/>
     </row>
     <row r="15" spans="1:143">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -3741,13 +3724,13 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="5"/>
-      <c r="AL15" s="65"/>
-      <c r="AM15" s="61"/>
-      <c r="AN15" s="61"/>
-      <c r="AO15" s="61"/>
-      <c r="AP15" s="61"/>
-      <c r="AQ15" s="61"/>
-      <c r="AR15" s="66"/>
+      <c r="AL15" s="4"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="5"/>
       <c r="AS15" s="4"/>
       <c r="AT15" s="1"/>
       <c r="AU15" s="1"/>
@@ -3874,7 +3857,7 @@
       <c r="EL15" s="5"/>
     </row>
     <row r="16" spans="1:143" ht="15" thickBot="1">
-      <c r="A16" s="39"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -3913,13 +3896,13 @@
       <c r="AI16" s="9"/>
       <c r="AJ16" s="9"/>
       <c r="AK16" s="13"/>
-      <c r="AL16" s="67"/>
-      <c r="AM16" s="68"/>
-      <c r="AN16" s="68"/>
-      <c r="AO16" s="68"/>
-      <c r="AP16" s="68"/>
-      <c r="AQ16" s="68"/>
-      <c r="AR16" s="69"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="9"/>
+      <c r="AN16" s="9"/>
+      <c r="AO16" s="9"/>
+      <c r="AP16" s="9"/>
+      <c r="AQ16" s="9"/>
+      <c r="AR16" s="13"/>
       <c r="AS16" s="15"/>
       <c r="AT16" s="9"/>
       <c r="AU16" s="9"/>
@@ -4020,7 +4003,7 @@
       <c r="EL16" s="13"/>
     </row>
     <row r="17" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -4061,13 +4044,13 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="5"/>
-      <c r="AL17" s="65"/>
-      <c r="AM17" s="61"/>
-      <c r="AN17" s="61"/>
-      <c r="AO17" s="61"/>
-      <c r="AP17" s="61"/>
-      <c r="AQ17" s="61"/>
-      <c r="AR17" s="66"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="5"/>
       <c r="AS17" s="4"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
@@ -4180,7 +4163,7 @@
       <c r="EL17" s="5"/>
     </row>
     <row r="18" spans="1:142" ht="15" thickBot="1">
-      <c r="A18" s="39"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
@@ -4219,13 +4202,13 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="5"/>
-      <c r="AL18" s="65"/>
-      <c r="AM18" s="61"/>
-      <c r="AN18" s="61"/>
-      <c r="AO18" s="61"/>
-      <c r="AP18" s="61"/>
-      <c r="AQ18" s="61"/>
-      <c r="AR18" s="66"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="5"/>
       <c r="AS18" s="4"/>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
@@ -4326,7 +4309,7 @@
       <c r="EL18" s="5"/>
     </row>
     <row r="19" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -4367,13 +4350,13 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="5"/>
-      <c r="AL19" s="65"/>
-      <c r="AM19" s="61"/>
-      <c r="AN19" s="61"/>
-      <c r="AO19" s="61"/>
-      <c r="AP19" s="61"/>
-      <c r="AQ19" s="61"/>
-      <c r="AR19" s="66"/>
+      <c r="AL19" s="4"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="5"/>
       <c r="AS19" s="4"/>
       <c r="AT19" s="1"/>
       <c r="AU19" s="1"/>
@@ -4480,7 +4463,7 @@
       <c r="EL19" s="5"/>
     </row>
     <row r="20" spans="1:142" ht="15" thickBot="1">
-      <c r="A20" s="48"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -4519,13 +4502,13 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="5"/>
-      <c r="AL20" s="65"/>
-      <c r="AM20" s="61"/>
-      <c r="AN20" s="61"/>
-      <c r="AO20" s="61"/>
-      <c r="AP20" s="61"/>
-      <c r="AQ20" s="61"/>
-      <c r="AR20" s="66"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="5"/>
       <c r="AS20" s="4"/>
       <c r="AT20" s="1"/>
       <c r="AU20" s="1"/>
@@ -4626,7 +4609,7 @@
       <c r="EL20" s="5"/>
     </row>
     <row r="21" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="48" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="21" t="s">
@@ -4667,13 +4650,13 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="5"/>
-      <c r="AL21" s="65"/>
-      <c r="AM21" s="61"/>
-      <c r="AN21" s="61"/>
-      <c r="AO21" s="61"/>
-      <c r="AP21" s="61"/>
-      <c r="AQ21" s="61"/>
-      <c r="AR21" s="66"/>
+      <c r="AL21" s="4"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="5"/>
       <c r="AS21" s="4"/>
       <c r="AT21" s="1"/>
       <c r="AU21" s="1"/>
@@ -4778,7 +4761,7 @@
       <c r="EL21" s="5"/>
     </row>
     <row r="22" spans="1:142" ht="15" thickBot="1">
-      <c r="A22" s="48"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
@@ -4817,13 +4800,13 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="5"/>
-      <c r="AL22" s="65"/>
-      <c r="AM22" s="61"/>
-      <c r="AN22" s="61"/>
-      <c r="AO22" s="61"/>
-      <c r="AP22" s="61"/>
-      <c r="AQ22" s="61"/>
-      <c r="AR22" s="66"/>
+      <c r="AL22" s="4"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="5"/>
       <c r="AS22" s="4"/>
       <c r="AT22" s="1"/>
       <c r="AU22" s="1"/>
@@ -4923,7 +4906,7 @@
       <c r="EL22" s="5"/>
     </row>
     <row r="23" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="21" t="s">
@@ -4964,13 +4947,13 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="5"/>
-      <c r="AL23" s="65"/>
-      <c r="AM23" s="61"/>
-      <c r="AN23" s="61"/>
-      <c r="AO23" s="61"/>
-      <c r="AP23" s="61"/>
-      <c r="AQ23" s="61"/>
-      <c r="AR23" s="66"/>
+      <c r="AL23" s="4"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="1"/>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="5"/>
       <c r="AS23" s="4"/>
       <c r="AT23" s="1"/>
       <c r="AU23" s="1"/>
@@ -5060,21 +5043,21 @@
       <c r="DI23" s="1"/>
       <c r="DJ23" s="5"/>
       <c r="DK23" s="4"/>
-      <c r="DL23" s="73"/>
-      <c r="DM23" s="73"/>
-      <c r="DN23" s="73"/>
-      <c r="DO23" s="73"/>
+      <c r="DL23" s="37"/>
+      <c r="DM23" s="37"/>
+      <c r="DN23" s="37"/>
+      <c r="DO23" s="37"/>
       <c r="DP23" s="1"/>
       <c r="DQ23" s="5"/>
       <c r="DR23" s="4"/>
-      <c r="DS23" s="73"/>
-      <c r="DT23" s="73"/>
-      <c r="DU23" s="73"/>
-      <c r="DV23" s="73"/>
+      <c r="DS23" s="37"/>
+      <c r="DT23" s="37"/>
+      <c r="DU23" s="37"/>
+      <c r="DV23" s="37"/>
       <c r="DW23" s="1"/>
       <c r="DX23" s="5"/>
-      <c r="DY23" s="65"/>
-      <c r="DZ23" s="61"/>
+      <c r="DY23" s="4"/>
+      <c r="DZ23" s="1"/>
       <c r="EA23" s="22">
         <v>5</v>
       </c>
@@ -5093,7 +5076,7 @@
       <c r="EL23" s="5"/>
     </row>
     <row r="24" spans="1:142" ht="15" thickBot="1">
-      <c r="A24" s="48"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
@@ -5132,13 +5115,13 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="5"/>
-      <c r="AL24" s="65"/>
-      <c r="AM24" s="61"/>
-      <c r="AN24" s="61"/>
-      <c r="AO24" s="61"/>
-      <c r="AP24" s="61"/>
-      <c r="AQ24" s="61"/>
-      <c r="AR24" s="66"/>
+      <c r="AL24" s="4"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="5"/>
       <c r="AS24" s="4"/>
       <c r="AT24" s="1"/>
       <c r="AU24" s="1"/>
@@ -5239,7 +5222,7 @@
       <c r="EL24" s="5"/>
     </row>
     <row r="25" spans="1:142" ht="14.5" customHeight="1">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="48" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="21" t="s">
@@ -5280,13 +5263,13 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="5"/>
-      <c r="AL25" s="65"/>
-      <c r="AM25" s="61"/>
-      <c r="AN25" s="61"/>
-      <c r="AO25" s="61"/>
-      <c r="AP25" s="61"/>
-      <c r="AQ25" s="61"/>
-      <c r="AR25" s="66"/>
+      <c r="AL25" s="4"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="5"/>
       <c r="AS25" s="4"/>
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
@@ -5403,7 +5386,7 @@
       <c r="EL25" s="5"/>
     </row>
     <row r="26" spans="1:142" ht="15" thickBot="1">
-      <c r="A26" s="48"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
@@ -5416,7 +5399,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="4"/>
       <c r="K26" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -5444,13 +5427,13 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="5"/>
-      <c r="AL26" s="65"/>
-      <c r="AM26" s="61"/>
-      <c r="AN26" s="61"/>
-      <c r="AO26" s="61"/>
-      <c r="AP26" s="61"/>
-      <c r="AQ26" s="61"/>
-      <c r="AR26" s="66"/>
+      <c r="AL26" s="4"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="5"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
@@ -5551,7 +5534,7 @@
       <c r="EL26" s="5"/>
     </row>
     <row r="27" spans="1:142" ht="15" customHeight="1">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -5592,13 +5575,13 @@
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="5"/>
-      <c r="AL27" s="65"/>
-      <c r="AM27" s="61"/>
-      <c r="AN27" s="61"/>
-      <c r="AO27" s="61"/>
-      <c r="AP27" s="61"/>
-      <c r="AQ27" s="61"/>
-      <c r="AR27" s="66"/>
+      <c r="AL27" s="4"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="5"/>
       <c r="AS27" s="4"/>
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
@@ -5701,7 +5684,7 @@
       <c r="EL27" s="11"/>
     </row>
     <row r="28" spans="1:142" ht="15" thickBot="1">
-      <c r="A28" s="47"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="8" t="s">
         <v>32</v>
       </c>
@@ -5740,13 +5723,13 @@
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
       <c r="AK28" s="8"/>
-      <c r="AL28" s="70"/>
-      <c r="AM28" s="71"/>
-      <c r="AN28" s="71"/>
-      <c r="AO28" s="71"/>
-      <c r="AP28" s="71"/>
-      <c r="AQ28" s="71"/>
-      <c r="AR28" s="72"/>
+      <c r="AL28" s="6"/>
+      <c r="AM28" s="7"/>
+      <c r="AN28" s="7"/>
+      <c r="AO28" s="7"/>
+      <c r="AP28" s="7"/>
+      <c r="AQ28" s="7"/>
+      <c r="AR28" s="8"/>
       <c r="AS28" s="6"/>
       <c r="AT28" s="7"/>
       <c r="AU28" s="7"/>
@@ -5848,6 +5831,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="DD3:DJ3"/>
+    <mergeCell ref="CW3:DC3"/>
+    <mergeCell ref="CP3:CV3"/>
+    <mergeCell ref="CI3:CO3"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="AL3:AR3"/>
+    <mergeCell ref="AE3:AK3"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="EF3:EL3"/>
     <mergeCell ref="DY3:EE3"/>
     <mergeCell ref="A7:A8"/>
@@ -5864,23 +5864,6 @@
     <mergeCell ref="AS3:AY3"/>
     <mergeCell ref="DR3:DX3"/>
     <mergeCell ref="DK3:DQ3"/>
-    <mergeCell ref="DD3:DJ3"/>
-    <mergeCell ref="CW3:DC3"/>
-    <mergeCell ref="CP3:CV3"/>
-    <mergeCell ref="CI3:CO3"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="AL3:AR3"/>
-    <mergeCell ref="AE3:AK3"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5892,8 +5875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FF6EFD-F608-4DA6-AB00-E35874012156}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="126" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -5902,81 +5885,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="53"/>
+      <c r="C3" s="55"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="59">
         <v>1</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="59"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="53"/>
+      <c r="C5" s="55"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="60">
         <v>45524</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="60"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="61">
         <v>45671</v>
       </c>
-      <c r="C7" s="59"/>
+      <c r="C7" s="61"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="53"/>
+      <c r="C8" s="55"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="56"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="26" t="s">
@@ -5994,7 +5977,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>57</v>
@@ -6005,7 +5988,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>57</v>
@@ -6016,7 +5999,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>57</v>
@@ -6027,7 +6010,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C19" s="35" t="s">
         <v>57</v>
@@ -6038,7 +6021,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>57</v>
@@ -6049,7 +6032,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C21" s="29" t="s">
         <v>57</v>
@@ -6060,7 +6043,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>57</v>
@@ -6071,7 +6054,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="29" t="s">
         <v>57</v>
@@ -6082,7 +6065,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>57</v>
@@ -6093,7 +6076,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C25" s="29" t="s">
         <v>57</v>
@@ -6104,7 +6087,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>57</v>
@@ -6115,7 +6098,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>57</v>
@@ -6126,7 +6109,7 @@
         <v>13</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C28" s="33" t="s">
         <v>57</v>
@@ -6137,7 +6120,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C29" s="35" t="s">
         <v>57</v>
@@ -6148,7 +6131,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>57</v>
@@ -6159,7 +6142,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C31" s="29" t="s">
         <v>57</v>
@@ -6170,7 +6153,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>57</v>
@@ -6181,7 +6164,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C33" s="29" t="s">
         <v>57</v>
@@ -6229,11 +6212,11 @@
       <c r="C38" s="28"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="26" t="s">
@@ -6262,7 +6245,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" s="29" t="s">
         <v>57</v>
@@ -6273,7 +6256,7 @@
         <v>3</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47" s="28" t="s">
         <v>57</v>
@@ -6306,7 +6289,7 @@
         <v>6</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="C50" s="29" t="s">
         <v>57</v>
@@ -6317,7 +6300,7 @@
         <v>7</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="28" t="s">
         <v>57</v>
@@ -6328,7 +6311,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>57</v>
@@ -6339,7 +6322,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C53" s="28" t="s">
         <v>57</v>
@@ -6350,7 +6333,7 @@
         <v>10</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C54" s="29" t="s">
         <v>57</v>

</xml_diff>